<commit_message>
8 columns with Part of Speech labels
</commit_message>
<xml_diff>
--- a/Ananse1/Ananse1.xlsx
+++ b/Ananse1/Ananse1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Akan\New Ananse Tales\Ananse1\Ananse1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F696E8E-4C47-47EC-AA41-DA546A2B008B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497F2240-3C1D-41E3-B6D8-A555F853A886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32865" yWindow="3855" windowWidth="22095" windowHeight="11055" xr2:uid="{02C65521-7DB8-4599-AFF3-A0D9D4E20026}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="760">
   <si>
     <t>AKAN</t>
   </si>
@@ -1489,6 +1489,861 @@
   </si>
   <si>
     <t>95 &lt;M’anansesem|NOUN&gt; &lt;a|PART&gt; &lt;metooye|VERB&gt; &lt;yi,|PRON&gt; &lt;se|SCONJ&gt; &lt;eye|VERB&gt; &lt;de|VERB&gt; &lt;o,|INTJ&gt; &lt;se|SCONJ&gt; &lt;ennye|VERB&gt; &lt;de|VERB&gt; &lt;o,|INTJ&gt; &lt;momfa|VERB&gt; &lt;bi|DET&gt; &lt;nko,|ADV&gt; &lt;na|CONJ&gt; &lt;momfa|VERB&gt; &lt;bi|DET&gt; &lt;mmera.|VERB&gt;</t>
+  </si>
+  <si>
+    <t>1  &lt;We|PRON&gt; &lt;do|AUX&gt; &lt;not|PART&gt; &lt;really|ADV&gt; &lt;mean|VERB&gt;, &lt;we|PRON&gt; &lt;do|AUX&gt; &lt;not|PART&gt; &lt;really|ADV&gt; &lt;mean|VERB&gt; &lt;(|PUNCT&gt; &lt;that|DET&gt; &lt;what|PRON&gt; &lt;we|PRON&gt; &lt;are|AUX&gt; &lt;going|VERB&gt; &lt;to|PART&gt; &lt;say|VERB&gt; &lt;is|AUX&gt; &lt;true|ADJ&gt;.|PUNCT</t>
+  </si>
+  <si>
+    <t>2  &lt;HOW|ADV&gt; &lt;KWAKU|PROPN&gt; &lt;ANANSE|PROPN&gt; &lt;THE|DET&gt; &lt;SPIDER|PROPN&gt; &lt;GOT|VERB&gt; &lt;ASO|PROPN&gt; &lt;IN|ADP&gt; &lt;MARRIAGE|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>3  &lt;THERE|ADV&gt; &lt;once|ADV&gt; &lt;lived|VERB&gt; &lt;a|DET&gt; &lt;certain|ADJ&gt; &lt;man|NOUN&gt; &lt;called|VERB&gt; &lt;Akwasi‐the‐jealous‐one|PROPN&gt;, &lt;and|CCONJ&gt; &lt;his|DET&gt; &lt;wife|NOUN&gt; &lt;was|AUX&gt; &lt;Aso|PROPN&gt;, &lt;and|CCONJ&gt; &lt;he|PRON&gt; &lt;did|AUX&gt; &lt;not|PART&gt; &lt;want|VERB&gt; &lt;anyone|PRON&gt; &lt;to|PART&gt; &lt;see|VERB&gt; &lt;Aso|PROPN&gt; &lt;or|CCONJ&gt; &lt;talk|VERB&gt; &lt;to|ADP&gt; &lt;her|PRON&gt;.|PUNCT</t>
+  </si>
+  <si>
+    <t>4  &lt;So|ADV&gt; &lt;he|PRON&gt; &lt;went|VERB&gt; &lt;and|CCONJ&gt; &lt;built|VERB&gt; &lt;a|DET&gt; &lt;small|ADJ&gt; &lt;settlement|NOUN&gt; &lt;for|ADP&gt; &lt;Aso|PROPN&gt; &lt;to|PART&gt; &lt;live|VERB&gt; &lt;in|ADP&gt;.|PUNCT</t>
+  </si>
+  <si>
+    <t>5  &lt;No|DET&gt; &lt;one|PRON&gt; &lt;ever|ADV&gt; &lt;went|VERB&gt; &lt;into|ADP&gt; &lt;the|DET&gt; &lt;village|NOUN&gt;.|PUNCT</t>
+  </si>
+  <si>
+    <t>6  &lt;Now|ADV&gt; &lt;he|PRON&gt;, &lt;Akwasi‐the‐jealous‐one|PROPN&gt;, &lt;could|AUX&gt; &lt;not|PART&gt; &lt;beget|VERB&gt; &lt;children|NOUN&gt;.|PUNCT</t>
+  </si>
+  <si>
+    <t>7  &lt;Because|SCONJ&gt; &lt;of|ADP&gt; &lt;that|DET&gt;, &lt;if|SCONJ&gt; &lt;he|PRON&gt; &lt;and|CCONJ&gt; &lt;his|DET&gt; &lt;wife|NOUN&gt; &lt;lived|VERB&gt; &lt;in|ADP&gt; &lt;town|NOUN&gt;, &lt;someone|PRON&gt; &lt;would|AUX&gt; &lt;take|VERB&gt; &lt;her|PRON&gt; &lt;away|ADV&gt;.|PUNCT</t>
+  </si>
+  <si>
+    <t>8  &lt;Now|ADV&gt; &lt;the|DET&gt; &lt;Sky‐god|PROPN&gt; &lt;told|VERB&gt; &lt;the|DET&gt; &lt;young|ADJ&gt; &lt;men|NOUN&gt;, &lt;saying|VERB&gt;, &lt;“Akwasi‐the‐jealous‐one|PROPN&gt; &lt;has|AUX&gt; &lt;been|AUX&gt; &lt;married|VERB&gt; &lt;to|ADP&gt; &lt;Aso|PROPN&gt; &lt;for|ADP&gt; &lt;a|DET&gt; &lt;very|ADV&gt; &lt;long|ADJ&gt; &lt;time|NOUN&gt;;|PUNCT&gt; &lt;she|PRON&gt; &lt;has|AUX&gt; &lt;not|PART&gt; &lt;conceived|VERB&gt; &lt;by|ADP&gt; &lt;him|PRON&gt; &lt;and|CCONJ&gt; &lt;borne|VERB&gt; &lt;a|DET&gt; &lt;child|NOUN&gt;, &lt;therefore|ADV&gt; &lt;he|PRON&gt; &lt;who|PRON&gt; &lt;is|AUX&gt; &lt;able|ADJ&gt;, &lt;let|VERB&gt; &lt;him|PRON&gt; &lt;go|VERB&gt; &lt;and|CCONJ&gt; &lt;take|VERB&gt; &lt;Aso|PROPN&gt;, &lt;and|CCONJ&gt; &lt;if|SCONJ&gt; &lt;she|PRON&gt; &lt;conceive|VERB&gt; &lt;by|ADP&gt; &lt;him|PRON&gt;, &lt;let|VERB&gt; &lt;him|PRON&gt; &lt;take|VERB&gt; &lt;her|PRON&gt;.”|PUNCT</t>
+  </si>
+  <si>
+    <t>9  &lt;All|DET&gt; &lt;the|DET&gt; &lt;young|ADJ&gt; &lt;men|NOUN&gt; &lt;tried|VERB&gt; &lt;their|DET&gt; &lt;best|ADJ&gt; &lt;to|PART&gt; &lt;lay|VERB&gt; &lt;hands|NOUN&gt; &lt;on|ADP&gt; &lt;her|PRON&gt;, &lt;but|CCONJ&gt; &lt;not|PART&gt; &lt;one|PRON&gt; &lt;was|AUX&gt; &lt;able|ADJ&gt;.|PUNCT</t>
+  </si>
+  <si>
+    <t>10 &lt;Kwaku|PROPN&gt; &lt;Ananse|PROPN&gt; &lt;was|AUX&gt; &lt;there|ADV&gt; &lt;watching|VERB&gt; &lt;these|DET&gt; &lt;events|NOUN&gt;, &lt;and|CCONJ&gt; &lt;he|PRON&gt; &lt;said|VERB&gt;, &lt;“I|PRON&gt; &lt;can|AUX&gt; &lt;go|VERB&gt; &lt;to|ADP&gt; &lt;Akwasi‐the‐jealous‐one’s|PROPN&gt; &lt;village.|NOUN&gt;”</t>
+  </si>
+  <si>
+    <t>11 &lt;The|DET&gt; &lt;Sky‐god|PROPN&gt; &lt;said|VERB&gt;, &lt;“Can|AUX&gt; &lt;you|PRON&gt; &lt;really|ADV&gt; &lt;do|VERB&gt; &lt;so|ADV&gt;?”|PUNCT</t>
+  </si>
+  <si>
+    <t>12 &lt;Ananse|PROPN&gt; &lt;said|VERB&gt;, &lt;“If|SCONJ&gt; &lt;you|PRON&gt; &lt;will|AUX&gt; &lt;give|VERB&gt; &lt;me|PRON&gt; &lt;what|PRON&gt; &lt;I|PRON&gt; &lt;require…|VERB&gt;</t>
+  </si>
+  <si>
+    <t>13 &lt;The|DET&gt; &lt;Sky‐god|PROPN&gt; &lt;asked|VERB&gt;, &lt;“What|PRON&gt; &lt;kind|NOUN&gt; &lt;of|ADP&gt; &lt;thing|NOUN&gt;?”|PUNCT</t>
+  </si>
+  <si>
+    <t>14 &lt;He|PRON&gt; &lt;said|VERB&gt;, &lt;“Medicine|NOUN&gt; &lt;for|ADP&gt; &lt;gun|NOUN&gt; &lt;and|CCONJ&gt; &lt;bullets.|NOUN&gt;”</t>
+  </si>
+  <si>
+    <t>15 &lt;And|CCONJ&gt; &lt;the|DET&gt; &lt;Sky‐god|PROPN&gt; &lt;gave|VERB&gt; &lt;them|PRON&gt; &lt;to|ADP&gt; &lt;him|PRON&gt;.|PUNCT</t>
+  </si>
+  <si>
+    <t>16 &lt;Then|ADV&gt; &lt;Ananse|PROPN&gt; &lt;took|VERB&gt; &lt;the|DET&gt; &lt;powder|NOUN&gt; &lt;and|CCONJ&gt; &lt;bullets|NOUN&gt; &lt;to|ADP&gt; &lt;various|ADJ&gt; &lt;small|ADJ&gt; &lt;villages|NOUN&gt;, &lt;saying|VERB&gt;, &lt;“The|DET&gt; &lt;Sky‐god|PROPN&gt; &lt;has|AUX&gt; &lt;bade|VERB&gt; &lt;me|PRON&gt; &lt;bring|VERB&gt; &lt;these|DET&gt; &lt;so|ADV&gt; &lt;you|PRON&gt; &lt;may|AUX&gt; &lt;kill|VERB&gt; &lt;meat;|NOUN&gt; &lt;when|SCONJ&gt; &lt;I|PRON&gt; &lt;return|VERB&gt;, &lt;I|PRON&gt; &lt;shall|AUX&gt; &lt;collect|VERB&gt; &lt;it|PRON&gt; &lt;and|CCONJ&gt; &lt;depart.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>17 &lt;He|PRON&gt; &lt;distributed|VERB&gt; &lt;the|DET&gt; &lt;powder|NOUN&gt; &lt;and|CCONJ&gt; &lt;bullets|NOUN&gt; &lt;among|ADP&gt; &lt;many|ADJ&gt; &lt;small|ADJ&gt; &lt;villages|NOUN&gt;, &lt;until|SCONJ&gt; &lt;all|DET&gt; &lt;were|AUX&gt; &lt;finished|VERB&gt;.|PUNCT</t>
+  </si>
+  <si>
+    <t>18 &lt;All|DET&gt; &lt;those|DET&gt; &lt;people|NOUN&gt; &lt;were|AUX&gt; &lt;able|ADJ&gt; &lt;to|PART&gt; &lt;kill|VERB&gt; &lt;some|DET&gt; &lt;animals|NOUN&gt;.|PUNCT</t>
+  </si>
+  <si>
+    <t>19 &lt;One|DET&gt; &lt;day|NOUN&gt;, &lt;Ananse|PROPN&gt; &lt;took|VERB&gt; &lt;a|DET&gt; &lt;palm‐leaf|ADJ&gt; &lt;basket,|NOUN&gt; &lt;as|SCONJ&gt; &lt;long|ADJ&gt; &lt;as|SCONJ&gt; &lt;from|ADP&gt; &lt;here|ADV&gt; &lt;to|ADP&gt; &lt;over|ADP&gt; &lt;yonder.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>20 &lt;He|PRON&gt; &lt;went|VERB&gt; &lt;back|ADV&gt; &lt;through|ADP&gt; &lt;the|DET&gt; &lt;villages|NOUN&gt; &lt;that|DET&gt; &lt;had|AUX&gt; &lt;used|VERB&gt; &lt;the|DET&gt; &lt;powder|NOUN&gt; &lt;and|CCONJ&gt; &lt;bullets,|NOUN&gt; &lt;gathering|VERB&gt; &lt;all|DET&gt; &lt;the|DET&gt; &lt;meat|NOUN&gt; &lt;they|PRON&gt; &lt;had|AUX&gt; &lt;killed.|VERB&gt;</t>
+  </si>
+  <si>
+    <t>English POS</t>
+  </si>
+  <si>
+    <t>21 &lt;Father|NOUN&gt; &lt;Ananse|PROPN&gt; &lt;carried|VERB&gt; &lt;the|DET&gt; &lt;meat|NOUN&gt; &lt;in|ADP&gt; &lt;the|DET&gt; &lt;palm‐leaf|ADJ&gt; &lt;basket|NOUN&gt; &lt;along|ADP&gt; &lt;the|DET&gt; &lt;path|NOUN&gt; &lt;leading|VERB&gt; &lt;to|ADP&gt; &lt;Akwasi‐the‐jealous‐one’s|PROPN&gt; &lt;settlement|NOUN&gt;.|PUNCT</t>
+  </si>
+  <si>
+    <t>22 &lt;When|SCONJ&gt; &lt;he|PRON&gt; &lt;arrived|VERB&gt; &lt;at|ADP&gt; &lt;the|DET&gt; &lt;stream|NOUN&gt; &lt;from|ADP&gt; &lt;which|DET&gt; &lt;Akwasi|PROPN&gt; &lt;and|CCONJ&gt; &lt;his|DET&gt; &lt;wife|NOUN&gt; &lt;drank|VERB&gt;, &lt;he|PRON&gt; &lt;picked|VERB&gt; &lt;out|PART&gt; &lt;some|DET&gt; &lt;meat|NOUN&gt; &lt;and|CCONJ&gt; &lt;put|VERB&gt; &lt;it|PRON&gt; &lt;in|ADP&gt;.|PUNCT</t>
+  </si>
+  <si>
+    <t>23 &lt;Ananse|PROPN&gt; &lt;strove|VERB&gt; &lt;hard|ADV&gt; &lt;to|PART&gt; &lt;place|VERB&gt; &lt;the|DET&gt; &lt;meat|NOUN&gt; &lt;in|ADP&gt; &lt;Akwasi‐the‐jealous‐one’s|PROPN&gt; &lt;water‐jar|NOUN&gt;.|PUNCT</t>
+  </si>
+  <si>
+    <t>24 &lt;And|CCONJ&gt; &lt;Aso|PROPN&gt; &lt;saw|VERB&gt; &lt;him|PRON&gt;.|PUNCT</t>
+  </si>
+  <si>
+    <t>25 &lt;She|PRON&gt; &lt;said|VERB&gt;, &lt;“Akwasi|PROPN&gt; &lt;e|INTJ&gt;! &lt;Come|VERB&gt; &lt;and|CCONJ&gt; &lt;look|VERB&gt; &lt;at|ADP&gt; &lt;something|PRON&gt; &lt;which|DET&gt; &lt;is|AUX&gt; &lt;coming|VERB&gt; &lt;into|ADP&gt; &lt;the|DET&gt; &lt;house|NOUN&gt; &lt;here|ADV&gt;, &lt;for|ADP&gt; &lt;what|PRON&gt; &lt;can|AUX&gt; &lt;it|PRON&gt; &lt;be|VERB&gt;?”|PUNCT</t>
+  </si>
+  <si>
+    <t>26 &lt;Ananse|PROPN&gt; &lt;said|VERB&gt;, &lt;“It’s|PRON&gt; &lt;the|DET&gt; &lt;Sky‐god|PROPN&gt; &lt;who|PRON&gt; &lt;is|AUX&gt; &lt;sending|VERB&gt; &lt;me|PRON&gt;, &lt;and|CCONJ&gt; &lt;I|PRON&gt; &lt;am|AUX&gt; &lt;weary|ADJ&gt;, &lt;and|CCONJ&gt; &lt;I|PRON&gt; &lt;am|AUX&gt; &lt;coming|VERB&gt; &lt;to|PART&gt; &lt;sleep|VERB&gt; &lt;here|ADV&gt;.”|PUNCT</t>
+  </si>
+  <si>
+    <t>27 &lt;Akwasi‐the‐jealous‐one|PROPN&gt; &lt;said|VERB&gt;, &lt;“I|PRON&gt; &lt;have|AUX&gt; &lt;heard|VERB&gt;, &lt;my|DET&gt; &lt;Lord’s|NOUN&gt; &lt;servant|NOUN&gt;.”|PUNCT</t>
+  </si>
+  <si>
+    <t>28 &lt;Aso|PROPN&gt; &lt;said|VERB&gt; &lt;to|ADP&gt; &lt;Ananse|PROPN&gt;, &lt;“Father|NOUN&gt; &lt;man|NOUN&gt;, &lt;some|DET&gt; &lt;of|ADP&gt; &lt;your|DET&gt; &lt;meat|NOUN&gt; &lt;has|AUX&gt; &lt;fallen|VERB&gt; &lt;down|ADV&gt; &lt;at|ADP&gt; &lt;the|DET&gt; &lt;main|ADJ&gt; &lt;entrance|NOUN&gt; &lt;to|ADP&gt; &lt;the|DET&gt; &lt;compound.|NOUN&gt;”|PUNCT</t>
+  </si>
+  <si>
+    <t>29 &lt;The|DET&gt; &lt;Spider|PROPN&gt; &lt;said|VERB&gt;, &lt;“Oh|INTJ&gt;, &lt;if|SCONJ&gt; &lt;you|PRON&gt; &lt;happen|VERB&gt; &lt;to|PART&gt; &lt;have|VERB&gt; &lt;a|DET&gt; &lt;dog|NOUN&gt;, &lt;let|VERB&gt; &lt;it|PRON&gt; &lt;go|VERB&gt; &lt;and|CCONJ&gt; &lt;take|VERB&gt; &lt;it|PRON&gt; &lt;and|CCONJ&gt; &lt;chew|VERB&gt; &lt;it.|PRON&gt;”</t>
+  </si>
+  <si>
+    <t>30 &lt;So|ADV&gt; &lt;Aso|PROPN&gt; &lt;went|VERB&gt; &lt;and|CCONJ&gt; &lt;got|VERB&gt; &lt;it|PRON&gt; &lt;and|CCONJ&gt; &lt;gave|VERB&gt; &lt;it|PRON&gt; &lt;to|ADP&gt; &lt;her|PRON&gt; &lt;husband|NOUN&gt;.|PUNCT</t>
+  </si>
+  <si>
+    <t>31 &lt;Then|ADV&gt; &lt;Ananse|PROPN&gt; &lt;said|VERB&gt;, &lt;“Mother|NOUN&gt;, &lt;set|VERB&gt; &lt;some|DET&gt; &lt;food|NOUN&gt; &lt;on|ADP&gt; &lt;the|DET&gt; &lt;fire|NOUN&gt; &lt;for|ADP&gt; &lt;me.|PRON&gt;”</t>
+  </si>
+  <si>
+    <t>32 &lt;Aso|PROPN&gt; &lt;put|VERB&gt; &lt;some|DET&gt; &lt;on|ADP&gt;, &lt;and|CCONJ&gt; &lt;Ananse|PROPN&gt; &lt;asked|VERB&gt;, &lt;“Mother|NOUN&gt;, &lt;is|AUX&gt; &lt;it|PRON&gt; &lt;fufuo|NOUN&gt; &lt;that|DET&gt; &lt;you|PRON&gt; &lt;are|AUX&gt; &lt;cooking|VERB&gt;, &lt;or|CCONJ&gt; &lt;eto?|NOUN&gt;”</t>
+  </si>
+  <si>
+    <t>33 &lt;Aso|PROPN&gt; &lt;replied|VERB&gt;, &lt;“Fufuo.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>34 &lt;Ananse|PROPN&gt; &lt;said|VERB&gt;, &lt;“Then|ADV&gt; &lt;it|PRON&gt; &lt;is|AUX&gt; &lt;too|ADV&gt; &lt;little;|ADJ&gt; &lt;go|VERB&gt; &lt;and|CCONJ&gt; &lt;fetch|VERB&gt; &lt;a|DET&gt; &lt;big|ADJ&gt; &lt;pot.|NOUN&gt;”</t>
+  </si>
+  <si>
+    <t>35 &lt;Aso|PROPN&gt; &lt;went|VERB&gt; &lt;and|CCONJ&gt; &lt;fetched|VERB&gt; &lt;a|DET&gt; &lt;big|ADJ&gt; &lt;one|PRON&gt;, &lt;and|CCONJ&gt; &lt;Ananse|PROPN&gt; &lt;said|VERB&gt;, &lt;“Come|VERB&gt; &lt;and|CCONJ&gt; &lt;get|VERB&gt; &lt;meat.|NOUN&gt;” &lt;There|ADV&gt; &lt;were|AUX&gt; &lt;forty|NUM&gt; &lt;hind‐quarters|NOUN&gt; &lt;of|ADP&gt; &lt;great|ADJ&gt; &lt;beasts.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>36 &lt;He|PRON&gt; &lt;said|VERB&gt;, &lt;“Take|VERB&gt; &lt;these|DET&gt; &lt;only|ADV&gt; &lt;and|CCONJ&gt; &lt;put|VERB&gt; &lt;them|PRON&gt; &lt;in,|ADP&gt; &lt;and|CCONJ&gt; &lt;if|SCONJ&gt; &lt;you|PRON&gt; &lt;had|AUX&gt; &lt;a|DET&gt; &lt;pot|NOUN&gt; &lt;big|ADJ&gt; &lt;enough,|ADV&gt; &lt;I|PRON&gt; &lt;would|AUX&gt; &lt;give|VERB&gt; &lt;you|PRON&gt; &lt;enough|ADJ&gt; &lt;meat|NOUN&gt; &lt;to|PART&gt; &lt;chew|VERB&gt; &lt;to|PART&gt; &lt;make|VERB&gt; &lt;your|DET&gt; &lt;teeth|NOUN&gt; &lt;fall|VERB&gt; &lt;out.|ADV&gt;”</t>
+  </si>
+  <si>
+    <t>37 &lt;Aso|PROPN&gt; &lt;finished|VERB&gt; &lt;preparing|VERB&gt; &lt;the|DET&gt; &lt;food,|NOUN&gt; &lt;turned|VERB&gt; &lt;it|PRON&gt; &lt;out|PART&gt; &lt;of|ADP&gt; &lt;the|DET&gt; &lt;pot,|NOUN&gt; &lt;and|CCONJ&gt; &lt;placed|VERB&gt; &lt;it|PRON&gt; &lt;on|ADP&gt; &lt;a|DET&gt; &lt;table,|NOUN&gt; &lt;splashed|VERB&gt; &lt;water,|NOUN&gt; &lt;and|CCONJ&gt; &lt;put|VERB&gt; &lt;it|PRON&gt; &lt;beside|ADP&gt; &lt;the|DET&gt; &lt;rest|NOUN&gt; &lt;of|ADP&gt; &lt;the|DET&gt; &lt;food.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>38 &lt;Then|ADV&gt; &lt;Aso|PROPN&gt; &lt;took|VERB&gt; &lt;her|DET&gt; &lt;portion|NOUN&gt; &lt;and|CCONJ&gt; &lt;went|VERB&gt; &lt;and|CCONJ&gt; &lt;sat|VERB&gt; &lt;near|ADP&gt; &lt;the|DET&gt; &lt;fire,|NOUN&gt; &lt;and|CCONJ&gt; &lt;the|DET&gt; &lt;men|NOUN&gt; &lt;went|VERB&gt; &lt;and|CCONJ&gt; &lt;sat|VERB&gt; &lt;down|ADV&gt; &lt;beside|ADP&gt; &lt;the|DET&gt; &lt;table.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>39 &lt;They|PRON&gt; &lt;touched|VERB&gt; &lt;the|DET&gt; &lt;backs|NOUN&gt; &lt;of|ADP&gt; &lt;each|DET&gt; &lt;other’s|DET&gt; &lt;hands|NOUN&gt; &lt;(|PUNCT&gt; &lt;i.e.|ADV&gt; &lt;ate|VERB&gt; &lt;from|ADP&gt; &lt;the|DET&gt; &lt;same|ADJ&gt; &lt;dish|NOUN&gt;|PUNCT).</t>
+  </si>
+  <si>
+    <t>40 &lt;All|DET&gt; &lt;the|DET&gt; &lt;time|NOUN&gt; &lt;they|PRON&gt; &lt;were|AUX&gt; &lt;eating|VERB&gt;, &lt;Kwaku|PROPN&gt; &lt;Ananse|PROPN&gt; &lt;said|VERB&gt;, &lt;“There|ADV&gt; &lt;is|AUX&gt; &lt;no|DET&gt; &lt;salt|NOUN&gt; &lt;in|ADP&gt; &lt;this|DET&gt; &lt;fufuo.|NOUN&gt;”</t>
+  </si>
+  <si>
+    <t>41 &lt;Akwasi|PROPN&gt; &lt;said|VERB&gt; &lt;to|ADP&gt; &lt;Aso|PROPN&gt;, &lt;“Bring|VERB&gt; &lt;some|DET&gt; &lt;salt.|NOUN&gt;”|PUNCT</t>
+  </si>
+  <si>
+    <t>42 &lt;But|CCONJ&gt; &lt;Ananse|PROPN&gt; &lt;said|VERB&gt;, &lt;“Not|PART&gt; &lt;at|ADP&gt; &lt;all,|ADV&gt; &lt;when|SCONJ&gt; &lt;the|DET&gt; &lt;woman|NOUN&gt; &lt;is|AUX&gt; &lt;eating,|VERB&gt; &lt;you|PRON&gt; &lt;cannot|AUX&gt; &lt;tell|VERB&gt; &lt;her|PRON&gt; &lt;to|PART&gt; &lt;get|VERB&gt; &lt;up|PART&gt; &lt;and|CCONJ&gt; &lt;bring|VERB&gt; &lt;salt,|NOUN&gt; &lt;do|AUX&gt; &lt;you|PRON&gt; &lt;yourself|PRON&gt; &lt;go|VERB&gt; &lt;and|CCONJ&gt; &lt;bring|VERB&gt; &lt;it.|PRON&gt;”</t>
+  </si>
+  <si>
+    <t>43 &lt;Akwasi|PROPN&gt; &lt;rose|VERB&gt; &lt;up,|ADV&gt; &lt;and|CCONJ&gt; &lt;Ananse|PROPN&gt; &lt;looked|VERB&gt; &lt;into|ADP&gt; &lt;his|DET&gt; &lt;bag,|NOUN&gt; &lt;took|VERB&gt; &lt;out|PART&gt; &lt;a|DET&gt; &lt;pinch|NOUN&gt; &lt;of|ADP&gt; &lt;purgative|ADJ&gt; &lt;medicine|NOUN&gt; &lt;and|CCONJ&gt; &lt;put|VERB&gt; &lt;it|PRON&gt; &lt;in|ADP&gt; &lt;the|DET&gt; &lt;fufuo.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>44 &lt;Then|ADV&gt; &lt;he|PRON&gt; &lt;called|VERB&gt; &lt;Akwasi,|PROPN&gt; &lt;saying,|VERB&gt; &lt;“Come,|VERB&gt; &lt;for|ADP&gt; &lt;I|PRON&gt; &lt;had|AUX&gt; &lt;brought|VERB&gt; &lt;some|DET&gt; &lt;with|ADP&gt; &lt;me.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>45 &lt;When|SCONJ&gt; &lt;Akwasi|PROPN&gt; &lt;came,|VERB&gt; &lt;Ananse|PROPN&gt; &lt;said,|VERB&gt; &lt;“Oh,|INTJ&gt; &lt;I|PRON&gt; &lt;shall|AUX&gt; &lt;eat|VERB&gt; &lt;no|DET&gt; &lt;more;|ADV&gt; &lt;I|PRON&gt; &lt;am|AUX&gt; &lt;full.”|ADJ&gt;</t>
+  </si>
+  <si>
+    <t>46 &lt;Akwasi,|PROPN&gt; &lt;who|PRON&gt; &lt;suspected|VERB&gt; &lt;nothing,|NOUN&gt; &lt;continued|VERB&gt; &lt;eating.|VERB&gt;</t>
+  </si>
+  <si>
+    <t>47 &lt;When|SCONJ&gt; &lt;they|PRON&gt; &lt;had|AUX&gt; &lt;finished|VERB&gt; &lt;eating,|VERB&gt; &lt;Akwasi|PROPN&gt; &lt;said,|VERB&gt; &lt;“Friend,|NOUN&gt; &lt;we|PRON&gt; &lt;are|AUX&gt; &lt;here|ADV&gt; &lt;with|ADP&gt; &lt;you,|PRON&gt; &lt;and|CCONJ&gt; &lt;yet|ADV&gt; &lt;we|PRON&gt; &lt;do|AUX&gt; &lt;not|PART&gt; &lt;know|VERB&gt; &lt;your|DET&gt; &lt;name.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>48 &lt;Ananse|PROPN&gt; &lt;replied,|VERB&gt; &lt;“I|PRON&gt; &lt;am|AUX&gt; &lt;called|VERB&gt; &lt;Rise‐up‐and‐make‐love‐to‐Aso.”|PROPN&gt;</t>
+  </si>
+  <si>
+    <t>49 &lt;Akwasi|PROPN&gt; &lt;said,|VERB&gt; &lt;“I|PRON&gt; &lt;have|AUX&gt; &lt;heard,|VERB&gt; &lt;and|CCONJ&gt; &lt;you,|PRON&gt; &lt;Aso,|PROPN&gt; &lt;have|AUX&gt; &lt;you|PRON&gt; &lt;heard|VERB&gt; &lt;this|DET&gt; &lt;man’s|NOUN&gt; &lt;name?”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>50 &lt;Aso|PROPN&gt; &lt;replied,|VERB&gt; &lt;“Yes,|INTJ&gt; &lt;I|PRON&gt; &lt;have|AUX&gt; &lt;heard.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>51 &lt;Akwasi|PROPN&gt; &lt;rose|VERB&gt; &lt;up|PART&gt; &lt;to|PART&gt; &lt;prepare|VERB&gt; &lt;one|DET&gt; &lt;of|ADP&gt; &lt;the|DET&gt; &lt;spare|ADJ&gt; &lt;bedrooms|NOUN&gt;, &lt;making|VERB&gt; &lt;all|DET&gt; &lt;comfortable.|ADJ&gt;</t>
+  </si>
+  <si>
+    <t>52 &lt;He|PRON&gt; &lt;said,|VERB&gt; &lt;“Rise‐up‐and‐make‐love‐to‐Aso,|PROPN&gt; &lt;this|DET&gt; &lt;is|AUX&gt; &lt;your|DET&gt; &lt;room,|NOUN&gt; &lt;go|VERB&gt; &lt;and|CCONJ&gt; &lt;sleep|VERB&gt; &lt;there.”|ADV&gt;</t>
+  </si>
+  <si>
+    <t>53 &lt;Ananse|PROPN&gt; &lt;said,|VERB&gt; &lt;“I|PRON&gt; &lt;am|AUX&gt; &lt;the|DET&gt; &lt;Soul‐washer|NOUN&gt; &lt;to|ADP&gt; &lt;the|DET&gt; &lt;Sky‐god,|PROPN&gt; &lt;and|CCONJ&gt; &lt;I|PRON&gt; &lt;sleep|VERB&gt; &lt;in|ADP&gt; &lt;an|DET&gt; &lt;open|ADJ&gt; &lt;veranda|NOUN&gt; &lt;room;|NOUN&gt; &lt;since|SCONJ&gt; &lt;my|DET&gt; &lt;mother|NOUN&gt; &lt;bore|VERB&gt; &lt;me|PRON&gt; &lt;and|CCONJ&gt; &lt;my|DET&gt; &lt;father|NOUN&gt; &lt;begat|VERB&gt; &lt;me,|PRON&gt; &lt;I|PRON&gt; &lt;have|AUX&gt; &lt;never|PART&gt; &lt;slept|VERB&gt; &lt;in|ADP&gt; &lt;a|DET&gt; &lt;closed|ADJ&gt; &lt;bedroom.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>54 &lt;Akwasi|PROPN&gt; &lt;asked,|VERB&gt; &lt;“Then|ADV&gt; &lt;where,|ADV&gt; &lt;then,|ADV&gt; &lt;will|AUX&gt; &lt;you|PRON&gt; &lt;sleep?”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>57 &lt;The|DET&gt; &lt;man|NOUN&gt; &lt;took|VERB&gt; &lt;out|PART&gt; &lt;a|DET&gt; &lt;sleeping‐mat|NOUN&gt; &lt;and|CCONJ&gt; &lt;laid|VERB&gt; &lt;it|PRON&gt; &lt;there|ADV&gt; &lt;for|ADP&gt; &lt;him.|PRON&gt;</t>
+  </si>
+  <si>
+    <t>58 &lt;Akwasi|PROPN&gt; &lt;and|CCONJ&gt; &lt;his|DET&gt; &lt;wife|NOUN&gt; &lt;went|VERB&gt; &lt;to|PART&gt; &lt;rest,|VERB&gt; &lt;and|CCONJ&gt; &lt;Ananse|PROPN&gt; &lt;also|ADV&gt; &lt;lay|VERB&gt; &lt;down|ADV&gt; &lt;there.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>59 &lt;Ananse|PROPN&gt; &lt;lay|VERB&gt; &lt;there|ADV&gt; &lt;and|CCONJ&gt; &lt;slipped|VERB&gt; &lt;in|ADP&gt; &lt;the|DET&gt; &lt;cross‐bar|NOUN&gt; &lt;of|ADP&gt; &lt;the|DET&gt; &lt;bedroom|NOUN&gt; &lt;door.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>60 &lt;Ananse|PROPN&gt; &lt;lay|VERB&gt; &lt;there|ADV&gt; &lt;and|CCONJ&gt; &lt;took|VERB&gt; &lt;his|DET&gt; &lt;musical|ADJ&gt; &lt;bow|NOUN&gt; &lt;(|PUNCT&gt; &lt;sepirewa|PROPN&gt;|PROPN&gt;) &lt;and|CCONJ&gt; &lt;sang|VERB&gt;:|PUNCT</t>
+  </si>
+  <si>
+    <t>61 &lt;Then|ADV&gt; &lt;he|PRON&gt; &lt;ceased|VERB&gt; &lt;playing|VERB&gt; &lt;his|DET&gt; &lt;sepirewa,|NOUN&gt; &lt;laid|VERB&gt; &lt;it|PRON&gt; &lt;aside,|ADV&gt; &lt;and|CCONJ&gt; &lt;lay|VERB&gt; &lt;down.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>63 &lt;Not|PART&gt; &lt;a|DET&gt; &lt;sound|NOUN&gt; &lt;in|ADP&gt; &lt;reply|NOUN&gt; &lt;(|PUNCT&gt; &lt;except|ADP&gt; &lt;the|DET&gt; &lt;chirping|NOUN&gt; &lt;of|ADP&gt; &lt;the|DET&gt; &lt;cicada|NOUN&gt;|PUNCT).|PUNCT</t>
+  </si>
+  <si>
+    <t>64 &lt;He|PRON&gt; &lt;called|VERB&gt; &lt;again,|ADV&gt; &lt;“Father|NOUN&gt; &lt;man.”|NOUN&gt; &lt;Still|ADV&gt; &lt;no|DET&gt; &lt;answer.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>65 &lt;The|DET&gt; &lt;medicine|NOUN&gt; &lt;had|AUX&gt; &lt;taken|VERB&gt; &lt;effect|NOUN&gt; &lt;on|ADP&gt; &lt;him,|PRON&gt; &lt;but|CCONJ&gt; &lt;he|PRON&gt; &lt;kept|VERB&gt; &lt;calling,|VERB&gt; &lt;“Father|NOUN&gt; &lt;man!”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>66 &lt;At|ADP&gt; &lt;last|ADV&gt; &lt;he|PRON&gt; &lt;said,|VERB&gt; &lt;“Rise-up-and-make-love-to-Aso.”|PROPN&gt;</t>
+  </si>
+  <si>
+    <t>67 &lt;The|DET&gt; &lt;Spider|PROPN&gt; &lt;said,|VERB&gt; &lt;“M!|INTJ&gt; &lt;M!|INTJ&gt; &lt;M!”|INTJ&gt;</t>
+  </si>
+  <si>
+    <t>68 &lt;He|PRON&gt; &lt;said,|VERB&gt; &lt;“Open|VERB&gt; &lt;the|DET&gt; &lt;door|NOUN&gt; &lt;for|ADP&gt; &lt;me.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>69 &lt;Ananse|PROPN&gt; &lt;opened|VERB&gt; &lt;it,|PRON&gt; &lt;and|CCONJ&gt; &lt;Akwasi|PROPN&gt; &lt;went|VERB&gt; &lt;off|ADV&gt; &lt;somewhere.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>70 &lt;Then|ADV&gt; &lt;Ananse|PROPN&gt; &lt;rose|VERB&gt; &lt;up|ADV&gt; &lt;and|CCONJ&gt; &lt;went|VERB&gt; &lt;into|ADP&gt; &lt;the|DET&gt; &lt;room|NOUN&gt; &lt;there.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>71 &lt;He|PRON&gt; &lt;said,|VERB&gt; &lt;“Aso,|PROPN&gt; &lt;did|AUX&gt; &lt;you|PRON&gt; &lt;hear|VERB&gt; &lt;what|PRON&gt; &lt;your|DET&gt; &lt;husband|NOUN&gt; &lt;said?”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>72 &lt;She|PRON&gt; &lt;replied,|VERB&gt; &lt;“What|PRON&gt; &lt;did|AUX&gt; &lt;he|PRON&gt; &lt;say?”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>73 &lt;He|PRON&gt; &lt;answered,|VERB&gt; &lt;“He|PRON&gt; &lt;said|VERB&gt; &lt;I|PRON&gt; &lt;must|AUX&gt; &lt;rise|VERB&gt; &lt;up|ADV&gt; &lt;and|CCONJ&gt; &lt;make|VERB&gt; &lt;love|NOUN&gt; &lt;to|ADP&gt; &lt;you.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>74 &lt;Aso|PROPN&gt; &lt;said,|VERB&gt; &lt;“You|PRON&gt; &lt;do|AUX&gt; &lt;not|PART&gt; &lt;lie.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>55 &lt;He|PRON&gt; &lt;replied,|VERB&gt; &lt;“Were|AUX&gt; &lt;I|PRON&gt; &lt;to|PART&gt; &lt;sleep|VERB&gt; &lt;in|ADP&gt; &lt;this|DET&gt; &lt;open|ADJ&gt; &lt;veranda|NOUN&gt; &lt;room,|NOUN&gt; &lt;that|DET&gt; &lt;would|AUX&gt; &lt;be|VERB&gt;56 &lt;Since|SCONJ&gt; &lt;I|PRON&gt; &lt;never|PART&gt; &lt;sleep|VERB&gt; &lt;in|ADP&gt; &lt;anyone’s|DET&gt; &lt;open|ADJ&gt; &lt;room|NOUN&gt; &lt;except|ADP&gt; &lt;that|DET&gt; &lt;of|ADP&gt; &lt;a|DET&gt; &lt;Sky‐god,|PROPN&gt; &lt;I|PRON&gt; &lt;shall|AUX&gt; &lt;just|ADV&gt; &lt;lie|VERB&gt; &lt;down|ADV&gt; &lt;in|ADP&gt; &lt;front|NOUN&gt; &lt;of|ADP&gt; &lt;this|DET&gt; &lt;closed|ADJ&gt; &lt;sleeping‐room|NOUN&gt; &lt;where|ADV&gt; &lt;you|PRON&gt; &lt;repose.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>75 &lt;Then|ADV&gt; &lt;he|PRON&gt; &lt;did|AUX&gt; &lt;it|PRON&gt; &lt;for|ADP&gt; &lt;her,|PRON&gt; &lt;and|CCONJ&gt; &lt;then|ADV&gt; &lt;he|PRON&gt; &lt;went|VERB&gt; &lt;and|CCONJ&gt; &lt;lay|VERB&gt; &lt;down|ADV&gt; &lt;again.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>76 &lt;That|DET&gt; &lt;night,|NOUN&gt; &lt;Akwasi|PROPN&gt; &lt;rose|VERB&gt; &lt;up|ADV&gt; &lt;nine|NUM&gt; &lt;times;|NOUN&gt; &lt;the|DET&gt; &lt;Spider|PROPN&gt; &lt;also|ADV&gt; &lt;went|VERB&gt; &lt;nine|NUM&gt; &lt;times|NOUN&gt; &lt;to|ADP&gt; &lt;Aso.|PROPN&gt;</t>
+  </si>
+  <si>
+    <t>77 &lt;Early|ADV&gt; &lt;the|DET&gt; &lt;next|ADJ&gt; &lt;morning,|NOUN&gt; &lt;Ananse|PROPN&gt; &lt;got|VERB&gt; &lt;up|ADV&gt; &lt;and|CCONJ&gt; &lt;left.|VERB&gt;</t>
+  </si>
+  <si>
+    <t>78 &lt;After|SCONJ&gt; &lt;about|ADV&gt; &lt;two|NUM&gt; &lt;moons,|NOUN&gt; &lt;Aso’s|PROPN&gt; &lt;belly|NOUN&gt; &lt;had|AUX&gt; &lt;grown|VERB&gt; &lt;quite|ADV&gt; &lt;large.|ADJ&gt;</t>
+  </si>
+  <si>
+    <t>79 &lt;Akwasi|PROPN&gt; &lt;questioned|VERB&gt; &lt;her,|PRON&gt; &lt;“Why|ADV&gt; &lt;has|AUX&gt; &lt;your|DET&gt; &lt;belly|NOUN&gt; &lt;got|VERB&gt; &lt;like|ADP&gt; &lt;this?|PRON&gt; &lt;Perhaps|ADV&gt; &lt;you|PRON&gt; &lt;are|AUX&gt; &lt;ill,|ADJ&gt; &lt;for|ADP&gt; &lt;I,|PRON&gt; &lt;who|PRON&gt; &lt;live|VERB&gt; &lt;with|ADP&gt; &lt;you,|PRON&gt; &lt;have|AUX&gt; &lt;no|DET&gt; &lt;child.|NOUN&gt;”</t>
+  </si>
+  <si>
+    <t>80 &lt;Aso|PROPN&gt; &lt;said,|VERB&gt; &lt;“You|PRON&gt; &lt;forgot|VERB&gt; &lt;the|DET&gt; &lt;man|NOUN&gt; &lt;who|PRON&gt; &lt;came|VERB&gt; &lt;here,|ADV&gt; &lt;whom|PRON&gt; &lt;you|PRON&gt; &lt;called|VERB&gt; &lt;‘Rise-up-and-make-love-to-Aso’?|PROPN&gt; &lt;He|PRON&gt; &lt;took|VERB&gt; &lt;me|PRON&gt; &lt;and|CCONJ&gt; &lt;I|PRON&gt; &lt;conceived|VERB&gt; &lt;by|ADP&gt; &lt;him.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>81 &lt;Akwasi-the-jealous-one|PROPN&gt; &lt;said,|VERB&gt; &lt;“Then|ADV&gt; &lt;get|VERB&gt; &lt;up;|ADV&gt; &lt;I|PRON&gt; &lt;shall|AUX&gt; &lt;take|VERB&gt; &lt;you|PRON&gt; &lt;to|ADP&gt; &lt;him.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>82 &lt;So|ADV&gt; &lt;they|PRON&gt; &lt;set|VERB&gt; &lt;out|PART&gt; &lt;for|ADP&gt; &lt;the|DET&gt; &lt;Sky-god’s|PROPN&gt; &lt;town.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>83 &lt;On|ADP&gt; &lt;the|DET&gt; &lt;way,|NOUN&gt; &lt;Aso|PROPN&gt; &lt;gave|VERB&gt; &lt;birth.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>84 &lt;When|SCONJ&gt; &lt;they|PRON&gt; &lt;reached|VERB&gt; &lt;the|DET&gt; &lt;Sky-god’s|PROPN&gt; &lt;place,|NOUN&gt; &lt;they|PRON&gt; &lt;told|VERB&gt; &lt;the|DET&gt; &lt;Sky-god|PROPN&gt; &lt;what|PRON&gt; &lt;had|AUX&gt; &lt;happened:|VERB&gt; &lt;“A|DET&gt; &lt;subject|NOUN&gt; &lt;of|ADP&gt; &lt;yours,|PRON&gt; &lt;whom|PRON&gt; &lt;you|PRON&gt; &lt;sent,|VERB&gt; &lt;slept|VERB&gt; &lt;at|ADP&gt; &lt;my|DET&gt; &lt;house,|NOUN&gt; &lt;and|CCONJ&gt; &lt;he|PRON&gt; &lt;took|VERB&gt; &lt;Aso,|PROPN&gt; &lt;and|CCONJ&gt; &lt;she|PRON&gt; &lt;conceived|VERB&gt; &lt;by|ADP&gt; &lt;him.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>85 &lt;The|DET&gt; &lt;Sky-god|PROPN&gt; &lt;said,|VERB&gt; &lt;“All|DET&gt; &lt;my|DET&gt; &lt;servants|NOUN&gt; &lt;are|AUX&gt; &lt;roofing|VERB&gt; &lt;the|DET&gt; &lt;huts;|NOUN&gt; &lt;go|VERB&gt; &lt;and|CCONJ&gt; &lt;point|VERB&gt; &lt;out|PART&gt; &lt;the|DET&gt; &lt;one|PRON&gt; &lt;you|PRON&gt; &lt;mean.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>86 &lt;They|PRON&gt; &lt;went,|VERB&gt; &lt;and|CCONJ&gt; &lt;there|ADV&gt; &lt;was|AUX&gt; &lt;Ananse|PROPN&gt; &lt;sitting|VERB&gt; &lt;on|ADP&gt; &lt;a|DET&gt; &lt;ridge|NOUN&gt; &lt;pole.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>87 &lt;Aso|PROPN&gt; &lt;said,|VERB&gt; &lt;“There|ADV&gt; &lt;he|PRON&gt; &lt;is.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>88 &lt;Then|ADV&gt; &lt;Ananse|PROPN&gt; &lt;ran|VERB&gt; &lt;and|CCONJ&gt; &lt;sat|VERB&gt; &lt;in|ADP&gt; &lt;the|DET&gt; &lt;middle.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>89 &lt;Again|ADV&gt; &lt;Aso|PROPN&gt; &lt;said,|VERB&gt; &lt;“There|ADV&gt; &lt;he|PRON&gt; &lt;is.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>90 &lt;Then|ADV&gt; &lt;Ananse|PROPN&gt; &lt;fell|VERB&gt; &lt;down|ADV&gt; &lt;from|ADP&gt; &lt;where|ADV&gt; &lt;he|PRON&gt; &lt;was|AUX&gt; &lt;sitting.|VERB&gt;</t>
+  </si>
+  <si>
+    <t>91 &lt;Now|ADV&gt; &lt;that|DET&gt; &lt;day|NOUN&gt; &lt;was|AUX&gt; &lt;Friday.|PROPN&gt;</t>
+  </si>
+  <si>
+    <t>92 &lt;Ananse|PROPN&gt; &lt;said,|VERB&gt; &lt;“I,|PRON&gt; &lt;who|PRON&gt; &lt;wash|VERB&gt; &lt;the|DET&gt; &lt;Sky-god’s|PROPN&gt; &lt;soul,|NOUN&gt; &lt;you|PRON&gt; &lt;have|AUX&gt; &lt;pointed|VERB&gt; &lt;your|DET&gt; &lt;hand|NOUN&gt; &lt;at|ADP&gt; &lt;me|PRON&gt;, &lt;causing|VERB&gt; &lt;me|PRON&gt; &lt;to|PART&gt; &lt;fall|VERB&gt; &lt;and|CCONJ&gt; &lt;get|VERB&gt; &lt;red|ADJ&gt; &lt;earth|NOUN&gt; &lt;on|ADP&gt; &lt;me.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>93 &lt;Immediately|ADV&gt; &lt;the|DET&gt; &lt;attendants|NOUN&gt; &lt;seized|VERB&gt; &lt;Akwasi-the-jealous-one,|PROPN&gt; &lt;and|CCONJ&gt; &lt;he|PRON&gt; &lt;was|AUX&gt; &lt;made|VERB&gt; &lt;to|PART&gt; &lt;sacrifice|VERB&gt; &lt;a|DET&gt; &lt;sheep.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>94 &lt;When|SCONJ&gt; &lt;Akwasi|PROPN&gt; &lt;had|AUX&gt; &lt;finished|VERB&gt; &lt;the|DET&gt; &lt;sacrifice,|NOUN&gt; &lt;he|PRON&gt; &lt;said|VERB&gt; &lt;to|ADP&gt; &lt;the|DET&gt; &lt;Sky-god,|PROPN&gt; &lt;“Here|ADV&gt; &lt;is|AUX&gt; &lt;the|DET&gt; &lt;woman;|NOUN&gt; &lt;let|VERB&gt; &lt;Ananse|PROPN&gt; &lt;take|VERB&gt; &lt;her.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>95 &lt;Ananse|PROPN&gt; &lt;took|VERB&gt; &lt;Aso;|PROPN&gt; &lt;but|CCONJ&gt; &lt;as|SCONJ&gt; &lt;for|ADP&gt; &lt;the|DET&gt; &lt;infant,|NOUN&gt; &lt;they|PRON&gt; &lt;killed|VERB&gt; &lt;it,|PRON&gt; &lt;cut|VERB&gt; &lt;it|PRON&gt; &lt;into|ADP&gt; &lt;pieces,|NOUN&gt; &lt;and|CCONJ&gt; &lt;scattered|VERB&gt; &lt;them|PRON&gt; &lt;about.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>96 &lt;That|DET&gt; &lt;is|AUX&gt; &lt;how|ADV&gt; &lt;jealousy|NOUN&gt; &lt;came|VERB&gt; &lt;among|ADP&gt; &lt;the|DET&gt; &lt;tribe.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>97 &lt;This|DET&gt; &lt;my|DET&gt; &lt;story,|NOUN&gt; &lt;which|PRON&gt; &lt;I|PRON&gt; &lt;have|AUX&gt; &lt;told,|VERB&gt; &lt;if|SCONJ&gt; &lt;it|PRON&gt; &lt;be|AUX&gt; &lt;sweet,|ADJ&gt; &lt;or|CCONJ&gt; &lt;if|SCONJ&gt; &lt;it|PRON&gt; &lt;be|AUX&gt; &lt;not|PART&gt; &lt;sweet,|ADJ&gt; &lt;take|VERB&gt; &lt;some|DET&gt; &lt;of|ADP&gt; &lt;it|PRON&gt; &lt;and|CCONJ&gt; &lt;leave|VERB&gt; &lt;the|DET&gt; &lt;rest,|NOUN&gt; &lt;or|CCONJ&gt; &lt;give|VERB&gt; &lt;me|PRON&gt; &lt;praise.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>1  &lt;Speak|VERB&gt; &lt;neg-say|VERB&gt;, &lt;neg-say|VERB&gt; &lt;oh|INTJ&gt;</t>
+  </si>
+  <si>
+    <t>2  &lt;HOW|ADV&gt; &lt;happen|VERB&gt; &lt;that|SCONJ&gt; &lt;Kwaku|PROPN&gt; &lt;Ananse|PROPN&gt; &lt;obtains|VERB&gt; &lt;Aso|PROPN&gt; &lt;marriage|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>3  &lt;A|DET&gt; &lt;certain|ADJ&gt; &lt;man|NOUN&gt; &lt;there|ADV&gt; &lt;was|AUX&gt; &lt;born|VERB&gt;, &lt;we-call|VERB&gt; &lt;him|PRON&gt; &lt;Akwasi|PROPN&gt; &lt;Jealous-one|PROPN&gt;, &lt;and|CCONJ&gt; &lt;his|DET&gt; &lt;wife|NOUN&gt; &lt;is|AUX&gt; &lt;Aso|PROPN&gt;, &lt;and|CCONJ&gt; &lt;he-not-want|VERB&gt; &lt;that|SCONJ&gt; &lt;someone|PRON&gt; &lt;see|VERB&gt; &lt;Aso|PROPN&gt;, &lt;or|CCONJ&gt; &lt;someone|PRON&gt; &lt;speak|VERB&gt; &lt;her|DET&gt; &lt;side|NOUN&gt;.</t>
+  </si>
+  <si>
+    <t>4  &lt;So|ADV&gt; &lt;he|PRON&gt; &lt;went|VERB&gt; &lt;tied|VERB&gt; &lt;settlement|NOUN&gt; &lt;for|ADP&gt; &lt;Aso|PROPN&gt; &lt;sit|VERB&gt;</t>
+  </si>
+  <si>
+    <t>5  &lt;Settlement|NOUN&gt; &lt;the|DET&gt; &lt;under|ADP&gt; &lt;nobody|PRON&gt; &lt;goes|VERB&gt; &lt;there|ADV&gt;.</t>
+  </si>
+  <si>
+    <t>6  &lt;He|PRON&gt; &lt;Akwasi|PROPN&gt; &lt;Jealous-one|PROPN&gt; &lt;is|AUX&gt; &lt;infertile|ADJ&gt;.</t>
+  </si>
+  <si>
+    <t>7  &lt;Because|SCONJ&gt; &lt;of|ADP&gt; &lt;that|DET&gt; &lt;he|PRON&gt; &lt;knows|VERB&gt; &lt;if|SCONJ&gt; &lt;he|PRON&gt; &lt;and|CCONJ&gt; &lt;her|PRON&gt; &lt;live|VERB&gt; &lt;town|NOUN&gt; &lt;inside|ADP&gt;, &lt;someone|PRON&gt; &lt;would-take|VERB&gt; &lt;her|PRON&gt;.</t>
+  </si>
+  <si>
+    <t>8  &lt;Sky-god|PROPN&gt; &lt;said|VERB&gt; &lt;told|VERB&gt; &lt;young-men|NOUN&gt; &lt;that|SCONJ&gt;, &lt;“Akwasi|PROPN&gt; &lt;Jealous-one|PROPN&gt; &lt;marry|VERB&gt; &lt;Aso|PROPN&gt; &lt;very-long-ago|ADV&gt;; &lt;she|PRON&gt; &lt;not-bear|VERB&gt; &lt;child|NOUN&gt;, &lt;so|SCONJ&gt; &lt;whoever|PRON&gt; &lt;can|AUX&gt; &lt;go|VERB&gt; &lt;take|VERB&gt; &lt;Aso|PROPN&gt; &lt;make|VERB&gt; &lt;her|PRON&gt; &lt;pregnant|ADJ&gt;, &lt;let|VERB&gt; &lt;him|PRON&gt; &lt;take|VERB&gt; &lt;her|PRON&gt;.”|PUNCT</t>
+  </si>
+  <si>
+    <t>9  &lt;The|DET&gt; &lt;young-men|NOUN&gt; &lt;all|DET&gt; &lt;tried|VERB&gt; &lt;effort|NOUN&gt; &lt;that|SCONJ&gt; &lt;our-hands|NOUN&gt; &lt;catch|VERB&gt; &lt;her|PRON&gt;, &lt;but|CCONJ&gt; &lt;nobody|PRON&gt; &lt;could|AUX&gt;.</t>
+  </si>
+  <si>
+    <t>10 &lt;Kwaku|PROPN&gt; &lt;Ananse|PROPN&gt; &lt;was|AUX&gt; &lt;there|ADV&gt;, &lt;he|PRON&gt; &lt;said|VERB&gt;, &lt;“I-able|VERB&gt; &lt;I-go|VERB&gt; &lt;Akwasi|PROPN&gt; &lt;Jealous-one|PROPN&gt; &lt;settlement.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>11 &lt;Sky-god|PROPN&gt; &lt;said,|VERB&gt; &lt;“Truly|ADV&gt;, &lt;you|PRON&gt; &lt;can?|AUX&gt;</t>
+  </si>
+  <si>
+    <t>12 &lt;Ananse|PROPN&gt; &lt;said,|VERB&gt; &lt;“Thing|NOUN&gt; &lt;I|PRON&gt; &lt;search,|VERB&gt; &lt;you|PRON&gt; &lt;must|AUX&gt; &lt;give|VERB&gt; &lt;me|PRON&gt; &lt;that|DET&gt; &lt;thing.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>13 &lt;Sky-god|PROPN&gt; &lt;said,|VERB&gt; &lt;“What?”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>14 &lt;He|PRON&gt; &lt;said,|VERB&gt; &lt;“Gun-powder|NOUN&gt; &lt;and|CCONJ&gt; &lt;bullets.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>15 &lt;And|CCONJ&gt; &lt;Sky-god|PROPN&gt; &lt;gave|VERB&gt; &lt;to|ADP&gt; &lt;him|PRON&gt;.</t>
+  </si>
+  <si>
+    <t>16 &lt;And|CCONJ&gt; &lt;Ananse|PROPN&gt; &lt;took|VERB&gt; &lt;gun-powder|NOUN&gt; &lt;and|CCONJ&gt; &lt;bullets|NOUN&gt; &lt;them|PRON&gt; &lt;went|VERB&gt; &lt;small-villages|NOUN&gt; &lt;saying,|VERB&gt; &lt;“Sky-god|PROPN&gt; &lt;says|VERB&gt; &lt;I|PRON&gt; &lt;bring|VERB&gt; &lt;gun-powder|NOUN&gt; &lt;and|CCONJ&gt; &lt;bullets|NOUN&gt; &lt;these|DET&gt; &lt;to|ADP&gt; &lt;you,|PRON&gt; &lt;that|SCONJ&gt; &lt;you|PRON&gt; &lt;kill|VERB&gt; &lt;meat,|NOUN&gt; &lt;and|CCONJ&gt; &lt;day|NOUN&gt; &lt;that|SCONJ&gt; &lt;I|PRON&gt; &lt;come|VERB&gt; &lt;here,|ADV&gt; &lt;I-will-take|VERB&gt; &lt;and|CCONJ&gt; &lt;go.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>17 &lt;He|PRON&gt; &lt;gave|VERB&gt; &lt;gun-powder|NOUN&gt; &lt;and|CCONJ&gt; &lt;bullets|NOUN&gt; &lt;to|ADP&gt; &lt;many|ADJ&gt; &lt;small-villages|NOUN&gt; &lt;till|SCONJ&gt; &lt;it|PRON&gt; &lt;finished.|VERB&gt;</t>
+  </si>
+  <si>
+    <t>18 &lt;People|NOUN&gt; &lt;all|DET&gt; &lt;got|VERB&gt; &lt;some|DET&gt; &lt;meat.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>19 &lt;One|DET&gt; &lt;day|NOUN&gt; &lt;Ananse|PROPN&gt; &lt;went|VERB&gt; &lt;took|VERB&gt; &lt;palm-leaf|ADJ&gt; &lt;basket,|NOUN&gt; &lt;Its|DET&gt; &lt;length|NOUN&gt; &lt;maybe|ADV&gt; &lt;from|ADP&gt; &lt;here|ADV&gt; &lt;to|ADP&gt; &lt;there.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>20 &lt;Ananse|PROPN&gt; &lt;took|VERB&gt; &lt;it|PRON&gt; &lt;went|VERB&gt; &lt;the|DET&gt; &lt;villages|NOUN&gt; &lt;he|PRON&gt; &lt;gave|VERB&gt; &lt;them|PRON&gt; &lt;gun-powder|NOUN&gt; &lt;and|CCONJ&gt; &lt;bullets,|NOUN&gt; &lt;went|VERB&gt; &lt;collected|VERB&gt; &lt;meat|NOUN&gt; &lt;they|PRON&gt; &lt;had|AUX&gt; &lt;killed|VERB&gt; &lt;all.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>AtoE POS</t>
+  </si>
+  <si>
+    <t>21 &lt;Father|NOUN&gt; &lt;Ananse|PROPN&gt; &lt;took|VERB&gt; &lt;that|DET&gt; &lt;meat|NOUN&gt; &lt;with|ADP&gt; &lt;the|DET&gt; &lt;basket,|NOUN&gt; &lt;set|VERB&gt; &lt;out,|PART&gt; &lt;and|CCONJ&gt; &lt;he|PRON&gt; &lt;arrived|VERB&gt; &lt;Akwasi|PROPN&gt; &lt;Jealous‐one|PROPN&gt; &lt;settlement|NOUN&gt; &lt;road|NOUN&gt; &lt;on.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>22 &lt;He|PRON&gt; &lt;arrived|VERB&gt; &lt;Akwasi|PROPN&gt; &lt;and|CCONJ&gt; &lt;that|DET&gt; &lt;woman|NOUN&gt; &lt;place|NOUN&gt; &lt;water|NOUN&gt; &lt;they|PRON&gt; &lt;drink|VERB&gt; &lt;inside,|ADV&gt; &lt;and|CCONJ&gt; &lt;he|PRON&gt; &lt;took|VERB&gt; &lt;some|DET&gt; &lt;meat|NOUN&gt; &lt;dropped.|VERB&gt;</t>
+  </si>
+  <si>
+    <t>23 &lt;Ananse|PROPN&gt; &lt;tried|VERB&gt; &lt;put|VERB&gt; &lt;the|DET&gt; &lt;basket|NOUN&gt; &lt;inside|ADP&gt; &lt;Akwasi|PROPN&gt; &lt;Jealous‐one|PROPN&gt; &lt;water‐jar.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>24 &lt;And|CCONJ&gt; &lt;Aso|PROPN&gt; &lt;saw|VERB&gt; &lt;him.|PRON&gt;</t>
+  </si>
+  <si>
+    <t>25 &lt;She|PRON&gt; &lt;said,|VERB&gt; &lt;“Akwasi|PROPN&gt; &lt;eh,|INTJ&gt; &lt;come|VERB&gt; &lt;see|VERB&gt; &lt;something|PRON&gt; &lt;that|SCONJ&gt; &lt;is|AUX&gt; &lt;coming|VERB&gt; &lt;house|NOUN&gt; &lt;here,|ADV&gt; &lt;what|PRON&gt; &lt;is|AUX&gt; &lt;it?”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>26 &lt;Ananse|PROPN&gt; &lt;said,|VERB&gt; &lt;“Sky‐god|PROPN&gt; &lt;who|PRON&gt; &lt;sends|VERB&gt; &lt;me,|PRON&gt; &lt;and|CCONJ&gt; &lt;I’m|PRON&gt; &lt;tired,|ADJ&gt; &lt;and|CCONJ&gt; &lt;I|PRON&gt; &lt;come|VERB&gt; &lt;sleep|VERB&gt; &lt;here.”|ADV&gt;</t>
+  </si>
+  <si>
+    <t>27 &lt;Akwasi|PROPN&gt; &lt;Jealous‐one|PROPN&gt; &lt;said,|VERB&gt; &lt;“I‐have‐heard,|VERB&gt; &lt;my|DET&gt; &lt;Lord’s|NOUN&gt; &lt;servant.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>28 &lt;Aso|PROPN&gt; &lt;said|VERB&gt; &lt;told|VERB&gt; &lt;Ananse|PROPN&gt; &lt;that,|SCONJ&gt; &lt;“Father|NOUN&gt; &lt;man,|NOUN&gt; &lt;your|DET&gt; &lt;meat|NOUN&gt; &lt;some|DET&gt; &lt;that|SCONJ&gt; &lt;parted|VERB&gt; &lt;dropped|VERB&gt; &lt;water‐jar.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>29 &lt;Ananse|PROPN&gt; &lt;said,|VERB&gt; &lt;“Oh,|INTJ&gt; &lt;if|SCONJ&gt; &lt;you|PRON&gt; &lt;have|VERB&gt; &lt;dog,|NOUN&gt; &lt;let|VERB&gt; &lt;it|PRON&gt; &lt;go|VERB&gt; &lt;take|VERB&gt; &lt;chew.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>30 &lt;And|CCONJ&gt; &lt;Aso|PROPN&gt; &lt;went|VERB&gt; &lt;took|VERB&gt; &lt;it,|PRON&gt; &lt;gave|VERB&gt; &lt;it|PRON&gt; &lt;to|ADP&gt; &lt;husband.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>31 &lt;Then|ADV&gt; &lt;Ananse|PROPN&gt; &lt;said,|VERB&gt; &lt;“Mother,|NOUN&gt; &lt;put|VERB&gt; &lt;food|NOUN&gt; &lt;on|ADP&gt; &lt;for|ADP&gt; &lt;me.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>32 &lt;Aso|PROPN&gt; &lt;put|VERB&gt; &lt;some,|DET&gt; &lt;and|CCONJ&gt; &lt;Ananse|PROPN&gt; &lt;said,|VERB&gt; &lt;“Mother,|NOUN&gt; &lt;is|AUX&gt; &lt;it|PRON&gt; &lt;fufuo|NOUN&gt; &lt;that|SCONJ&gt; &lt;you|PRON&gt; &lt;cook,|VERB&gt; &lt;or|CCONJ&gt; &lt;eto?”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>33 &lt;Aso|PROPN&gt; &lt;said,|VERB&gt; &lt;“Fufuo.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>34 &lt;Ananse|PROPN&gt; &lt;said,|VERB&gt; &lt;“Then|ADV&gt; &lt;it’s|PRON&gt; &lt;small;|ADJ&gt; &lt;go|VERB&gt; &lt;bring|VERB&gt; &lt;pot|NOUN&gt; &lt;big.”|ADJ&gt;</t>
+  </si>
+  <si>
+    <t>35 &lt;Aso|PROPN&gt; &lt;went|VERB&gt; &lt;took|VERB&gt; &lt;big,|ADJ&gt; &lt;and|CCONJ&gt; &lt;Ananse|PROPN&gt; &lt;said,|VERB&gt; &lt;“Come|VERB&gt; &lt;take|VERB&gt; &lt;meat.”|NOUN&gt; &lt;There|ADV&gt; &lt;huge|ADJ&gt; &lt;animals|NOUN&gt; &lt;hind‐quarters|NOUN&gt; &lt;forty.|NUM&gt;</t>
+  </si>
+  <si>
+    <t>36 &lt;He|PRON&gt; &lt;said,|VERB&gt; &lt;“Take|VERB&gt; &lt;these|DET&gt; &lt;only|ADV&gt; &lt;put|VERB&gt; &lt;inside,|ADP&gt; &lt;and|CCONJ&gt; &lt;if|SCONJ&gt; &lt;you|PRON&gt; &lt;had|AUX&gt; &lt;pot|NOUN&gt; &lt;big,|ADJ&gt; &lt;then|ADV&gt; &lt;I|PRON&gt; &lt;give|VERB&gt; &lt;you|PRON&gt; &lt;chew|VERB&gt; &lt;meat|NOUN&gt; &lt;make|VERB&gt; &lt;your|DET&gt; &lt;teeth|NOUN&gt; &lt;fall.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>37 &lt;Aso|PROPN&gt; &lt;finished|VERB&gt; &lt;the|DET&gt; &lt;food,|NOUN&gt; &lt;poured|VERB&gt; &lt;it|PRON&gt; &lt;out,|PART&gt; &lt;put|VERB&gt; &lt;on|ADP&gt; &lt;table,|NOUN&gt; &lt;poured|VERB&gt; &lt;water|NOUN&gt; &lt;placed|VERB&gt; &lt;there.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>38 &lt;And|CCONJ&gt; &lt;Aso|PROPN&gt; &lt;took|VERB&gt; &lt;her|DET&gt; &lt;portion|NOUN&gt; &lt;went|VERB&gt; &lt;near|ADP&gt; &lt;fire,|NOUN&gt; &lt;and|CCONJ&gt; &lt;men|NOUN&gt; &lt;they|PRON&gt; &lt;went|VERB&gt; &lt;sat|VERB&gt; &lt;table|NOUN&gt; &lt;side.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>39 &lt;And|CCONJ&gt; &lt;we|PRON&gt; &lt;touched|VERB&gt; &lt;our‐hands|NOUN&gt; &lt;backs.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>40 &lt;We|PRON&gt; &lt;eat,|VERB&gt; &lt;we|PRON&gt; &lt;eat,|VERB&gt; &lt;Kwaku|PROPN&gt; &lt;Ananse|PROPN&gt; &lt;said,|VERB&gt; &lt;“This|DET&gt; &lt;fufuo,|NOUN&gt; &lt;salt|NOUN&gt; &lt;not|PART&gt; &lt;in.”|ADP&gt;</t>
+  </si>
+  <si>
+    <t>41 &lt;Akwasi|PROPN&gt; &lt;said|VERB&gt; &lt;to|ADP&gt; &lt;Aso,|PROPN&gt; &lt;“Bring|VERB&gt; &lt;some.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>43 &lt;Akwasi|PROPN&gt; &lt;rose,|VERB&gt; &lt;and|CCONJ&gt; &lt;Ananse|PROPN&gt; &lt;searched|VERB&gt; &lt;his|DET&gt; &lt;bag|NOUN&gt; &lt;then|ADV&gt; &lt;took|VERB&gt; &lt;purgative|ADJ&gt; &lt;medicine|NOUN&gt; &lt;put|VERB&gt; &lt;in|ADP&gt; &lt;fufuo.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>44 &lt;Then|ADV&gt; &lt;he|PRON&gt; &lt;called|VERB&gt; &lt;Akwasi|PROPN&gt; &lt;that,|SCONJ&gt; &lt;“Come|VERB&gt; &lt;for|ADP&gt; &lt;the|DET&gt; &lt;salt|NOUN&gt; &lt;I|PRON&gt; &lt;brought.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>45 &lt;Akwasi|PROPN&gt; &lt;came,|VERB&gt; &lt;Ananse|PROPN&gt; &lt;said,|VERB&gt; &lt;“Oh,|INTJ&gt; &lt;I|PRON&gt; &lt;not|PART&gt; &lt;eat|VERB&gt; &lt;more,|ADV&gt; &lt;I’m|PRON&gt; &lt;full.”|ADJ&gt;</t>
+  </si>
+  <si>
+    <t>46 &lt;Akwasi|PROPN&gt; &lt;who|PRON&gt; &lt;not|PART&gt; &lt;suspect|VERB&gt; &lt;anything,|NOUN&gt; &lt;continued|VERB&gt; &lt;eating,|VERB&gt; &lt;he|PRON&gt; &lt;ate|VERB&gt; &lt;and|CCONJ&gt; &lt;ate.|VERB&gt;</t>
+  </si>
+  <si>
+    <t>47 &lt;We|PRON&gt; &lt;finished|VERB&gt; &lt;eating,|VERB&gt; &lt;and|CCONJ&gt; &lt;Akwasi|PROPN&gt; &lt;said,|VERB&gt; &lt;“Friend,|NOUN&gt; &lt;we|PRON&gt; &lt;and|CCONJ&gt; &lt;you|PRON&gt; &lt;sit|VERB&gt; &lt;here,|ADV&gt; &lt;yet|ADV&gt; &lt;we|PRON&gt; &lt;not|PART&gt; &lt;know|VERB&gt; &lt;your|DET&gt; &lt;name.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>51 &lt;Akwasi|PROPN&gt; &lt;rose|VERB&gt; &lt;went|VERB&gt; &lt;prepared|VERB&gt; &lt;bedroom|NOUN&gt; &lt;one|DET&gt; &lt;nicely.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>54 &lt;Akwasi|PROPN&gt; &lt;said,|VERB&gt; &lt;“Where|ADV&gt; &lt;then|ADV&gt; &lt;you|PRON&gt; &lt;sleep?”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>56 &lt;The|DET&gt; &lt;man|NOUN&gt; &lt;took|VERB&gt; &lt;mat|NOUN&gt; &lt;placed|VERB&gt; &lt;it|PRON&gt; &lt;there.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>57 &lt;Akwasi|PROPN&gt; &lt;and|CCONJ&gt; &lt;his|DET&gt; &lt;wife|NOUN&gt; &lt;went|VERB&gt; &lt;slept,|VERB&gt; &lt;and|CCONJ&gt; &lt;Ananse|PROPN&gt; &lt;also|ADV&gt; &lt;lay|VERB&gt; &lt;there.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>58 &lt;Ananse|PROPN&gt; &lt;lay|VERB&gt; &lt;there|ADV&gt; &lt;and|CCONJ&gt; &lt;parted|VERB&gt; &lt;mouth|NOUN&gt; &lt;wide.|ADJ&gt; &lt;Ananse|PROPN&gt; &lt;lay|VERB&gt; &lt;there|ADV&gt; &lt;took|VERB&gt; &lt;his|DET&gt; &lt;sepirewa|NOUN&gt; &lt;said:|VERB&gt;</t>
+  </si>
+  <si>
+    <t>60 &lt;Then|ADV&gt; &lt;he|PRON&gt; &lt;stopped|VERB&gt; &lt;sepirewa,|NOUN&gt; &lt;and|CCONJ&gt; &lt;placed|VERB&gt; &lt;it|PRON&gt; &lt;there|ADV&gt; &lt;and|CCONJ&gt; &lt;he|PRON&gt; &lt;slept.|VERB&gt;</t>
+  </si>
+  <si>
+    <t>42 &lt;But|CCONJ&gt; &lt;Ananse|PROPN&gt; &lt;said,|VERB&gt; &lt;“No,|INTJ&gt; &lt;woman|NOUN&gt; &lt;is|AUX&gt; &lt;eating,|VERB&gt; &lt;you|PRON&gt; &lt;say|VERB&gt; &lt;get-up|VERB&gt; &lt;go|VERB&gt; &lt;bring|VERB&gt; &lt;salt,|NOUN&gt; &lt;you|PRON&gt; &lt;self|NOUN&gt; &lt;get-up|VERB&gt; &lt;go|VERB&gt; &lt;bring|VERB&gt; &lt;come.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>48 &lt;Ananse|PROPN&gt; &lt;said,|VERB&gt; &lt;“My|DET&gt; &lt;name|NOUN&gt; &lt;is|AUX&gt; &lt;Rise-up-and-make-love-to-Aso.”|PROPN&gt;</t>
+  </si>
+  <si>
+    <t>49 &lt;Akwasi|PROPN&gt; &lt;said,|VERB&gt; &lt;“I-have-heard,|VERB&gt; &lt;Aso,|PROPN&gt; &lt;you-have-heard|VERB&gt; &lt;this|DET&gt; &lt;man|NOUN&gt; &lt;name?”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>50 &lt;Aso|PROPN&gt; &lt;said,|VERB&gt; &lt;“Yes,|INTJ&gt; &lt;I-have-heard.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>52 &lt;He|PRON&gt; &lt;said,|VERB&gt; &lt;“Rise-up-and-make-love-to-Aso,|PROPN&gt; &lt;your|DET&gt; &lt;bedroom|NOUN&gt; &lt;here,|ADV&gt; &lt;go|VERB&gt; &lt;sleep|VERB&gt; &lt;there.”|ADV&gt;</t>
+  </si>
+  <si>
+    <t>53 &lt;Ananse|PROPN&gt; &lt;said,|VERB&gt; &lt;“Sky-god’s|PROPN&gt; &lt;soul|NOUN&gt; &lt;washer|NOUN&gt; &lt;is|AUX&gt; &lt;me,|PRON&gt; &lt;I|PRON&gt; &lt;sleep|VERB&gt; &lt;veranda,|NOUN&gt; &lt;since|SCONJ&gt; &lt;mother|NOUN&gt; &lt;father|NOUN&gt; &lt;gave|VERB&gt; &lt;birth|NOUN&gt; &lt;me,|PRON&gt; &lt;I|PRON&gt; &lt;never|PART&gt; &lt;slept|VERB&gt; &lt;closed|ADJ&gt; &lt;bedroom.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>55 &lt;He|PRON&gt; &lt;said,|VERB&gt; &lt;“If|SCONJ&gt; &lt;I|PRON&gt; &lt;lie|VERB&gt; &lt;this|DET&gt; &lt;open|ADJ&gt; &lt;veranda,|NOUN&gt; &lt;then|ADV&gt; &lt;it|PRON&gt; &lt;means|VERB&gt; &lt;you|PRON&gt; &lt;and|CCONJ&gt; &lt;your|DET&gt; &lt;Sky-god|PROPN&gt; &lt;are|AUX&gt; &lt;same,|ADJ&gt; &lt;it|PRON&gt; &lt;shows|VERB&gt; &lt;I|PRON&gt; &lt;lie|VERB&gt; &lt;Sky-god|PROPN&gt; &lt;open|ADJ&gt; &lt;veranda.|NOUN&gt; &lt;I|PRON&gt; &lt;never|PART&gt; &lt;lie|VERB&gt; &lt;anyone|PRON&gt; &lt;open|ADJ&gt; &lt;veranda|NOUN&gt; &lt;except|ADP&gt; &lt;Sky-god,|PROPN&gt; &lt;so|SCONJ&gt; &lt;closed|ADJ&gt; &lt;bedroom|NOUN&gt; &lt;that|DET&gt; &lt;you|PRON&gt; &lt;sleep|VERB&gt; &lt;front|ADV&gt; &lt;is|AUX&gt; &lt;where|ADV&gt; &lt;I|PRON&gt; &lt;sleep.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>59 &lt;“Akuamoa|PROPN&gt; &lt;Ananse,|PROPN&gt; &lt;today|ADV&gt; &lt;we-will-do|VERB&gt; &lt;something|NOUN&gt; &lt;today.|ADV&gt; &lt;Nyame|PROPN&gt; &lt;own,|ADJ&gt; &lt;Nsia|PROPN&gt; &lt;child|NOUN&gt; &lt;Ananse,|PROPN&gt; &lt;today|ADV&gt; &lt;we-will-do|VERB&gt; &lt;something|NOUN&gt; &lt;today.|ADV&gt; &lt;Nyame|PROPN&gt; &lt;soul-washer|NOUN&gt; &lt;Ananse,|PROPN&gt; &lt;today|ADV&gt; &lt;I-see|VERB&gt; &lt;something.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>61 &lt;He|PRON&gt; &lt;sleeps|VERB&gt; &lt;small,|ADV&gt; &lt;he|PRON&gt; &lt;hears|VERB&gt; &lt;Akwasi|PROPN&gt; &lt;Jealous-one|PROPN&gt; &lt;calling|VERB&gt; &lt;him,|PRON&gt; &lt;“Father|NOUN&gt; &lt;man.”|NOUN&gt; &lt;Silence!|INTJ&gt;</t>
+  </si>
+  <si>
+    <t>62 &lt;“Father|NOUN&gt; &lt;man.”|NOUN&gt; &lt;Silence!|INTJ&gt;</t>
+  </si>
+  <si>
+    <t>63 &lt;Akwasi|PROPN&gt; &lt;Jealous-one|PROPN&gt; &lt;is|AUX&gt; &lt;dying;|VERB&gt; &lt;medicine|NOUN&gt; &lt;has|AUX&gt; &lt;him,|PRON&gt; &lt;yet|ADV&gt; &lt;he|PRON&gt; &lt;calls|VERB&gt; &lt;“Father|NOUN&gt; &lt;man.”|NOUN&gt; &lt;Silence!|INTJ&gt;</t>
+  </si>
+  <si>
+    <t>64 &lt;Then|ADV&gt; &lt;he|PRON&gt; &lt;said,|VERB&gt; &lt;“Rise-up-and-make-love-to-Aso.”|PROPN&gt;</t>
+  </si>
+  <si>
+    <t>65 &lt;He|PRON&gt; &lt;said,|VERB&gt; &lt;“M!|INTJ&gt; &lt;M!|INTJ&gt; &lt;M!”|INTJ&gt;</t>
+  </si>
+  <si>
+    <t>66 &lt;He|PRON&gt; &lt;said,|VERB&gt; &lt;“Open|VERB&gt; &lt;me.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>67 &lt;Ananse|PROPN&gt; &lt;opened,|VERB&gt; &lt;and|CCONJ&gt; &lt;Akwasi|PROPN&gt; &lt;went|VERB&gt; &lt;somewhere.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>68 &lt;Then|ADV&gt; &lt;Ananse|PROPN&gt; &lt;rose|VERB&gt; &lt;went|VERB&gt; &lt;bedroom|NOUN&gt; &lt;there.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>69 &lt;He|PRON&gt; &lt;said,|VERB&gt; &lt;“Aso,|PROPN&gt; &lt;you|PRON&gt; &lt;heard|VERB&gt; &lt;what|PRON&gt; &lt;your|DET&gt; &lt;husband|NOUN&gt; &lt;said?”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>70 &lt;She|PRON&gt; &lt;said,|VERB&gt; &lt;“He|PRON&gt; &lt;said|VERB&gt; &lt;what?”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>71 &lt;He|PRON&gt; &lt;said,|VERB&gt; &lt;“He|PRON&gt; &lt;said|VERB&gt; &lt;me|PRON&gt; &lt;rise|VERB&gt; &lt;I|PRON&gt; &lt;take|VERB&gt; &lt;you.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>72 &lt;Aso|PROPN&gt; &lt;said,|VERB&gt; &lt;“You|PRON&gt; &lt;are|AUX&gt; &lt;not|PART&gt; &lt;lying.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>73 &lt;Then|ADV&gt; &lt;he|PRON&gt; &lt;did|VERB&gt; &lt;for|ADP&gt; &lt;her,|PRON&gt; &lt;then|ADV&gt; &lt;returned|VERB&gt; &lt;lay|VERB&gt; &lt;down.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>74 &lt;Night|NOUN&gt; &lt;that,|PRON&gt; &lt;Akwasi|PROPN&gt; &lt;rose|VERB&gt; &lt;nine|NUM&gt; &lt;times;|NOUN&gt; &lt;Ananse|PROPN&gt; &lt;also|ADV&gt; &lt;went|VERB&gt; &lt;Aso|PROPN&gt; &lt;side|NOUN&gt; &lt;nine|NUM&gt; &lt;times.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>75 &lt;Early|ADV&gt; &lt;morning,|NOUN&gt; &lt;Ananse|PROPN&gt; &lt;set|VERB&gt; &lt;out|PART&gt; &lt;left.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>76 &lt;After|SCONJ&gt; &lt;maybe|ADV&gt; &lt;two|NUM&gt; &lt;months,|NOUN&gt; &lt;Aso|PROPN&gt; &lt;belly|NOUN&gt; &lt;has|AUX&gt; &lt;grown|VERB&gt; &lt;bigger.|ADJ&gt;</t>
+  </si>
+  <si>
+    <t>77 &lt;Akwasi|PROPN&gt; &lt;asked|VERB&gt; &lt;her|PRON&gt; &lt;that,|SCONJ&gt; &lt;“Why|ADV&gt; &lt;that|DET&gt; &lt;your|DET&gt; &lt;belly|NOUN&gt; &lt;grown|VERB&gt; &lt;so|ADV&gt; &lt;big,|ADJ&gt; &lt;maybe|ADV&gt; &lt;you|PRON&gt; &lt;sickness,|NOUN&gt; &lt;and|CCONJ&gt; &lt;me|PRON&gt; &lt;who|PRON&gt; &lt;with|ADP&gt; &lt;you,|PRON&gt; &lt;I|PRON&gt; &lt;not|PART&gt; &lt;have|VERB&gt; &lt;child.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>78 &lt;Aso|PROPN&gt; &lt;said,|VERB&gt; &lt;“You|PRON&gt; &lt;forgot|VERB&gt; &lt;the|DET&gt; &lt;man|NOUN&gt; &lt;who|PRON&gt; &lt;came|VERB&gt; &lt;here|ADV&gt; &lt;who|PRON&gt; &lt;you|PRON&gt; &lt;called|VERB&gt; &lt;‘Rise-up-and-make-love-to-Aso’?|PROPN&gt; &lt;He|PRON&gt; &lt;is|AUX&gt; &lt;the|DET&gt; &lt;one|PRON&gt; &lt;who|PRON&gt; &lt;took|VERB&gt; &lt;me|PRON&gt; &lt;and|CCONJ&gt; &lt;made|VERB&gt; &lt;me|PRON&gt; &lt;conceive.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>79 &lt;Akwasi|PROPN&gt; &lt;Jealous-one|PROPN&gt; &lt;said,|VERB&gt; &lt;“Rise|VERB&gt; &lt;let|VERB&gt; &lt;me|PRON&gt; &lt;take|VERB&gt; &lt;you|PRON&gt; &lt;go|VERB&gt; &lt;to|ADP&gt; &lt;him.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>80 &lt;We|PRON&gt; &lt;went|VERB&gt; &lt;Sky-god|PROPN&gt; &lt;town.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>81 &lt;On|ADP&gt; &lt;the|DET&gt; &lt;road|NOUN&gt; &lt;Aso|PROPN&gt; &lt;gave|VERB&gt; &lt;birth.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>82 &lt;We|PRON&gt; &lt;reached|VERB&gt; &lt;Nyame’s|PROPN&gt; &lt;town|NOUN&gt; &lt;told|VERB&gt; &lt;Nyame|PROPN&gt; &lt;matters|NOUN&gt; &lt;that,|SCONJ&gt; &lt;“Your|DET&gt; &lt;servant|NOUN&gt; &lt;one|PRON&gt; &lt;who|PRON&gt; &lt;you|PRON&gt; &lt;sent|VERB&gt; &lt;who|PRON&gt; &lt;slept|VERB&gt; &lt;my|DET&gt; &lt;house,|NOUN&gt; &lt;he|PRON&gt; &lt;took|VERB&gt; &lt;Aso|PROPN&gt; &lt;and|CCONJ&gt; &lt;impregnated|VERB&gt; &lt;her.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>83 &lt;Sky-god|PROPN&gt; &lt;said,|VERB&gt; &lt;“My|DET&gt; &lt;servants|NOUN&gt; &lt;all|DET&gt; &lt;roofing|VERB&gt; &lt;huts,|NOUN&gt; &lt;go|VERB&gt; &lt;show|VERB&gt; &lt;man|NOUN&gt; &lt;single.”|ADJ&gt;</t>
+  </si>
+  <si>
+    <t>84 &lt;We|PRON&gt; &lt;went,|VERB&gt; &lt;and|CCONJ&gt; &lt;Ananse|PROPN&gt; &lt;sits|VERB&gt; &lt;on|ADP&gt; &lt;ridge-pole.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>85 &lt;Aso|PROPN&gt; &lt;said,|VERB&gt; &lt;“There|ADV&gt; &lt;he|PRON&gt; &lt;is.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>86 &lt;Then|ADV&gt; &lt;Ananse|PROPN&gt; &lt;jumped|VERB&gt; &lt;sat|VERB&gt; &lt;middle.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>87 &lt;And|CCONJ&gt; &lt;Aso|PROPN&gt; &lt;again|ADV&gt; &lt;said,|VERB&gt; &lt;“There|ADV&gt; &lt;he|PRON&gt; &lt;is.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>88 &lt;Then|ADV&gt; &lt;Ananse|PROPN&gt; &lt;from|ADP&gt; &lt;top|ADJ&gt; &lt;place|NOUN&gt; &lt;fell|VERB&gt; &lt;ground.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>89 &lt;Day|NOUN&gt; &lt;that|DET&gt; &lt;on,|ADV&gt; &lt;it|PRON&gt; &lt;is|AUX&gt; &lt;Friday.|PROPN&gt;</t>
+  </si>
+  <si>
+    <t>90 &lt;Ananse|PROPN&gt; &lt;said,|VERB&gt; &lt;“Me|PRON&gt; &lt;wash|VERB&gt; &lt;soul|NOUN&gt; &lt;and|CCONJ&gt; &lt;you|PRON&gt; &lt;put|VERB&gt; &lt;your|DET&gt; &lt;hand|NOUN&gt; &lt;on|ADP&gt; &lt;me|PRON&gt; &lt;that|SCONJ&gt; &lt;I|PRON&gt; &lt;fell|VERB&gt; &lt;red|ADJ&gt; &lt;earth|NOUN&gt; &lt;on|ADP&gt; &lt;me.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>91 &lt;Then|ADV&gt; &lt;immediately|ADV&gt; &lt;attendants|NOUN&gt; &lt;seized|VERB&gt; &lt;Akwasi|PROPN&gt; &lt;Jealous-one,|PROPN&gt; &lt;and|CCONJ&gt; &lt;he|PRON&gt; &lt;slaughtered|VERB&gt; &lt;sheep.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>92 &lt;Akwasi|PROPN&gt; &lt;Jealous-one|PROPN&gt; &lt;slaughtered|VERB&gt; &lt;sheep|NOUN&gt; &lt;finished,|ADV&gt; &lt;he|PRON&gt; &lt;said|VERB&gt; &lt;to|ADP&gt; &lt;Sky-god,|PROPN&gt; &lt;“Woman|NOUN&gt; &lt;this|DET&gt; &lt;is,|VERB&gt; &lt;let|VERB&gt; &lt;Ananse|PROPN&gt; &lt;take|VERB&gt; &lt;her.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>93 &lt;Ananse|PROPN&gt; &lt;took|VERB&gt; &lt;Aso,|PROPN&gt; &lt;and|CCONJ&gt; &lt;the|DET&gt; &lt;infant|NOUN&gt; &lt;they|PRON&gt; &lt;killed|VERB&gt; &lt;it|PRON&gt; &lt;cut|VERB&gt; &lt;its|DET&gt; &lt;flesh|NOUN&gt; &lt;scattered|VERB&gt; &lt;them|PRON&gt; &lt;about.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>94 &lt;That|DET&gt; &lt;is|AUX&gt; &lt;how|ADV&gt; &lt;jealousy|NOUN&gt; &lt;will|AUX&gt; &lt;come|VERB&gt; &lt;tribe.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>95 &lt;My|DET&gt; &lt;Ananse|PROPN&gt; &lt;tale|NOUN&gt; &lt;that|SCONJ&gt; &lt;I|PRON&gt; &lt;told|VERB&gt; &lt;this,|PRON&gt; &lt;if|SCONJ&gt; &lt;it|PRON&gt; &lt;good|ADJ&gt; &lt;oh,|INTJ&gt; &lt;if|SCONJ&gt; &lt;it|PRON&gt; &lt;not|PART&gt; &lt;good|ADJ&gt; &lt;oh,|INTJ&gt; &lt;take|VERB&gt; &lt;some|DET&gt; &lt;go,|ADV&gt; &lt;and|CCONJ&gt; &lt;take|VERB&gt; &lt;some|DET&gt; &lt;bring.|VERB&gt;</t>
+  </si>
+  <si>
+    <t>1  &lt;Y?|PRON&gt; &lt;nse|NOUN&gt; &lt;ankasa,|ADV&gt; &lt;nse|NOUN&gt; &lt;ankasa|ADV&gt; &lt;o|INTJ&gt;</t>
+  </si>
+  <si>
+    <t>2  &lt;Ey?|VERB&gt; &lt;d?n|PRON&gt; &lt;a|PART&gt; &lt;Kwaku|PROPN&gt; &lt;Ananse|PROPN&gt; &lt;nya|VERB&gt; &lt;Aso|PROPN&gt; &lt;aware|VERB&gt;</t>
+  </si>
+  <si>
+    <t>3  &lt;?w?|VERB&gt; &lt;barima|NOUN&gt; &lt;bi|DET&gt; &lt;a|PART&gt; &lt;yew?|VERB&gt; &lt;no,|PRON&gt; &lt;y?fr?|VERB&gt; &lt;no|PRON&gt; &lt;Akwasi|PROPN&gt; &lt;Ninkunfuo,|PROPN&gt; &lt;na|CONJ&gt; &lt;ne|DET&gt; &lt;yere|NOUN&gt; &lt;y?|AUX&gt; &lt;Aso,|PROPN&gt; &lt;na|CONJ&gt; &lt;wannp?|VERB&gt; &lt;s?|SCONJ&gt; &lt;obi|PRON&gt; &lt;hu|VERB&gt; &lt;Aso,|PROPN&gt; &lt;anaa|CONJ&gt; &lt;obi|PRON&gt; &lt;kasa|VERB&gt; &lt;ne|DET&gt; &lt;ho.|PRON&gt;</t>
+  </si>
+  <si>
+    <t>4  &lt;Enti|ADV&gt; &lt;?k??|VERB&gt; &lt;b??|VERB&gt; &lt;akura|NOUN&gt; &lt;maa|VERB&gt; &lt;Aso|PROPN&gt; &lt;tena|VERB&gt;</t>
+  </si>
+  <si>
+    <t>5  &lt;Kurow|NOUN&gt; &lt;no|DET&gt; &lt;ase,|NOUN&gt; &lt;obi|PRON&gt; &lt;nko|ADV&gt; &lt;h?|ADV&gt;</t>
+  </si>
+  <si>
+    <t>6  &lt;?no|PRON&gt; &lt;Akwasi|PROPN&gt; &lt;Ninkunfuo|PROPN&gt; &lt;y?|AUX&gt; &lt;onipa|NOUN&gt; &lt;a|PART&gt; &lt;onwo|VERB&gt; &lt;ba|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>7  &lt;Esiane|ADV&gt; &lt;saa|ADV&gt; &lt;nti|ADP&gt; &lt;onim|VERB&gt; &lt;s?|SCONJ&gt; &lt;s?|SCONJ&gt; &lt;?ne|PRON&gt; &lt;no|PRON&gt; &lt;te|VERB&gt; &lt;kurom’,|NOUN&gt; &lt;obi|PRON&gt; &lt;b?fa|VERB&gt; &lt;no|PRON&gt;</t>
+  </si>
+  <si>
+    <t>8  &lt;Nyankop?n|PROPN&gt; &lt;kae|VERB&gt; &lt;kyer?|VERB&gt; &lt;mmerante|NOUN&gt; &lt;no|DET&gt; &lt;se,|SCONJ&gt; &lt;“Akwasi|PROPN&gt; &lt;Ninkunfuo|PROPN&gt; &lt;aware|VERB&gt; &lt;Aso|PROPN&gt; &lt;f?f??f?;|ADJ&gt; &lt;na|CONJ&gt; &lt;wanhyia|VERB&gt; &lt;ba,|NOUN&gt; &lt;enti|ADV&gt; &lt;obiara|PRON&gt; &lt;a|PART&gt; &lt;obetumi|VERB&gt; &lt;ak?fa|VERB&gt; &lt;no|PRON&gt; &lt;ama|VERB&gt; &lt;onyam,|NOUN&gt; &lt;onfa|VERB&gt; &lt;no.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>9  &lt;Mmerante|NOUN&gt; &lt;no|DET&gt; &lt;nyinaa|PRON&gt; &lt;boaboa|VERB&gt; &lt;mmoden|NOUN&gt; &lt;s?|SCONJ&gt; &lt;y?n|PRON&gt; &lt;nsa|NOUN&gt; &lt;nka|VERB&gt; &lt;no,|PRON&gt; &lt;nanso|CONJ&gt; &lt;obi|PRON&gt; &lt;antumi|VERB&gt;</t>
+  </si>
+  <si>
+    <t>10 &lt;Kwaku|PROPN&gt; &lt;Ananse|PROPN&gt; &lt;te|VERB&gt; &lt;h?,|ADV&gt; &lt;?kae|VERB&gt; &lt;se,|SCONJ&gt; &lt;“Metumi|AUX&gt; &lt;ak?|VERB&gt; &lt;Akwasi|PROPN&gt; &lt;Ninkunfuo|PROPN&gt; &lt;akurase.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>11 &lt;Nyame|PROPN&gt; &lt;bisaa|VERB&gt; &lt;se,|SCONJ&gt; &lt;“Ampa?|INTJ&gt; &lt;Wobetumi|VERB&gt; &lt;anaa?”|PART&gt;</t>
+  </si>
+  <si>
+    <t>12 &lt;Ananse|PROPN&gt; &lt;kae|VERB&gt; &lt;se,|SCONJ&gt; &lt;“Biribi|PRON&gt; &lt;a|PART&gt; &lt;meresr?,|VERB&gt; &lt;s?|SCONJ&gt; &lt;wode|VERB&gt; &lt;ma|VERB&gt; &lt;me|PRON&gt; &lt;a.”|PART&gt;</t>
+  </si>
+  <si>
+    <t>13 &lt;Nyame|PROPN&gt; &lt;bisaa|VERB&gt; &lt;se,|SCONJ&gt; &lt;“D?n?”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>14 &lt;?see,|VERB&gt; &lt;“Atuduro|NOUN&gt; &lt;ne|CONJ&gt; &lt;ab?|NOUN&gt; &lt;(aboo).”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>15 &lt;Na|CONJ&gt; &lt;Nyame|PROPN&gt; &lt;de|VERB&gt; &lt;maa|VERB&gt; &lt;no|PRON&gt;</t>
+  </si>
+  <si>
+    <t>16 &lt;Na|CONJ&gt; &lt;Ananse|PROPN&gt; &lt;faa|VERB&gt; &lt;atuduro|NOUN&gt; &lt;ne|CONJ&gt; &lt;ab?|NOUN&gt; &lt;no|PRON&gt; &lt;k??|VERB&gt; &lt;nkuraa|NOUN&gt; &lt;ketewa|ADJ&gt; &lt;te|VERB&gt; &lt;se,|SCONJ&gt; &lt;“Nyame|PROPN&gt; &lt;se|SCONJ&gt; &lt;memfa|VERB&gt; &lt;atuduro|NOUN&gt; &lt;ne|CONJ&gt; &lt;ab?|NOUN&gt; &lt;yi|PRON&gt; &lt;mmr?|VERB&gt; &lt;mo,|PRON&gt; &lt;na|CONJ&gt; &lt;mo|PRON&gt; &lt;nkum|VERB&gt; &lt;nam,|NOUN&gt; &lt;na|CONJ&gt; &lt;da|NOUN&gt; &lt;a|PART&gt; &lt;m?ba|VERB&gt; &lt;ha|ADV&gt; &lt;no,|PRON&gt; &lt;mefa|VERB&gt; &lt;ak?.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>17 &lt;?maa|VERB&gt; &lt;nkuraa|NOUN&gt; &lt;pii|ADJ&gt; &lt;atuduro|NOUN&gt; &lt;ne|CONJ&gt; &lt;ab?,|NOUN&gt; &lt;kosi|VERB&gt; &lt;s?|SCONJ&gt; &lt;?sae|VERB&gt;</t>
+  </si>
+  <si>
+    <t>18 &lt;Nnipa|NOUN&gt; &lt;no|DET&gt; &lt;nyinaa|PRON&gt; &lt;nyaa|VERB&gt; &lt;nam|NOUN&gt; &lt;bi|DET&gt;</t>
+  </si>
+  <si>
+    <t>19 &lt;Da|NOUN&gt; &lt;koro|ADJ&gt; &lt;bi,|DET&gt; &lt;Ananse|PROPN&gt; &lt;k?faa|VERB&gt; &lt;bede|NOUN&gt; &lt;(apalapala|ADJ&gt; &lt;ky?n),|NOUN&gt; &lt;ne|DET&gt; &lt;tenten|ADJ&gt; &lt;b?y?|VERB&gt; &lt;te|VERB&gt; &lt;s?|SCONJ&gt; &lt;fi|NOUN&gt; &lt;ha|ADV&gt; &lt;k?|VERB&gt; &lt;h?|ADV&gt;</t>
+  </si>
+  <si>
+    <t>20 &lt;Ananse|PROPN&gt; &lt;de|VERB&gt; &lt;no|PRON&gt; &lt;k??|VERB&gt; &lt;nkuraa|NOUN&gt; &lt;a|PART&gt; &lt;?maa|VERB&gt; &lt;w?n|PRON&gt; &lt;atuduro|NOUN&gt; &lt;ne|CONJ&gt; &lt;ab?|NOUN&gt; &lt;no,|PRON&gt; &lt;k?|VERB&gt; &lt;boaboa|VERB&gt; &lt;nam|NOUN&gt; &lt;a|PART&gt; &lt;wokum|VERB&gt; &lt;nyinaa|PRON&gt;</t>
+  </si>
+  <si>
+    <t>EtoA POS</t>
+  </si>
+  <si>
+    <t>21 &lt;Agya|NOUN&gt; &lt;Ananse|PROPN&gt; &lt;faa|VERB&gt; &lt;nam|NOUN&gt; &lt;no|PRON&gt; &lt;ne|DET&gt; &lt;bede|NOUN&gt; &lt;no|PRON&gt; &lt;so,|ADV&gt; &lt;na|CONJ&gt; &lt;?faa|VERB&gt; &lt;kwan|NOUN&gt; &lt;k?duruu|VERB&gt; &lt;Akwasi|PROPN&gt; &lt;Ninkunfuo|PROPN&gt; &lt;akuraa|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>22 &lt;?duruu|VERB&gt; &lt;asuo|NOUN&gt; &lt;a|PART&gt; &lt;Akwasi|PROPN&gt; &lt;ne|DET&gt; &lt;ne|DET&gt; &lt;yere|NOUN&gt; &lt;nom|VERB&gt; &lt;mu,|PRON&gt; &lt;na|CONJ&gt; &lt;?wiei|VERB&gt; &lt;nam|NOUN&gt; &lt;bi|DET&gt; &lt;guu|VERB&gt; &lt;mu|ADV&gt;</t>
+  </si>
+  <si>
+    <t>23 &lt;Ananse|PROPN&gt; &lt;boaboa|VERB&gt; &lt;mmoden|NOUN&gt; &lt;de|VERB&gt; &lt;bede|NOUN&gt; &lt;no|PRON&gt; &lt;guu|VERB&gt; &lt;Akwasi|PROPN&gt; &lt;Ninkunfuo|PROPN&gt; &lt;ntwonom’|NOUN&gt; &lt;mu|ADV&gt;</t>
+  </si>
+  <si>
+    <t>24 &lt;Na|CONJ&gt; &lt;Aso|PROPN&gt; &lt;huu|VERB&gt; &lt;no|PRON&gt;</t>
+  </si>
+  <si>
+    <t>25 &lt;?kae|VERB&gt; &lt;se,|SCONJ&gt; &lt;“Akwasi|PROPN&gt; &lt;e,|INTJ&gt; &lt;bra|VERB&gt; &lt;hw?|VERB&gt; &lt;biribi|PRON&gt; &lt;a|PART&gt; &lt;?ba|VERB&gt; &lt;fie|NOUN&gt; &lt;yi,|PRON&gt; &lt;na|CONJ&gt; &lt;d?n?”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>26 &lt;Ananse|PROPN&gt; &lt;kae|VERB&gt; &lt;se,|SCONJ&gt; &lt;“Nyame|PROPN&gt; &lt;na|CONJ&gt; &lt;wasoma|VERB&gt; &lt;me,|PRON&gt; &lt;na|CONJ&gt; &lt;mabere,|VERB&gt; &lt;na|CONJ&gt; &lt;m?da|VERB&gt; &lt;ha.”|ADV&gt;</t>
+  </si>
+  <si>
+    <t>27 &lt;Akwasi|PROPN&gt; &lt;Ninkunfuo|PROPN&gt; &lt;se,|VERB&gt; &lt;“Mate,|VERB&gt; &lt;me|PRON&gt; &lt;wura|NOUN&gt; &lt;akoa.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>28 &lt;Aso|PROPN&gt; &lt;ka|VERB&gt; &lt;kyer??|VERB&gt; &lt;Ananse|PROPN&gt; &lt;se,|SCONJ&gt; &lt;“Agya|NOUN&gt; &lt;barima,|NOUN&gt; &lt;wo|PRON&gt; &lt;nam|NOUN&gt; &lt;no|PRON&gt; &lt;bi|DET&gt; &lt;agu|VERB&gt; &lt;ntwonom’|NOUN&gt; &lt;no|PRON&gt; &lt;mu.”|ADV&gt;</t>
+  </si>
+  <si>
+    <t>29 &lt;Ananse|PROPN&gt; &lt;see,|VERB&gt; &lt;“O,|INTJ&gt; &lt;s?|SCONJ&gt; &lt;wo|PRON&gt; &lt;w?|VERB&gt; &lt;kraman|NOUN&gt; &lt;bi|DET&gt; &lt;a,|SCONJ&gt; &lt;ma|VERB&gt; &lt;no|PRON&gt; &lt;nko|ADV&gt; &lt;fa|VERB&gt; &lt;nwe.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>30 &lt;Na|CONJ&gt; &lt;Aso|PROPN&gt; &lt;k?faa|VERB&gt; &lt;de|VERB&gt; &lt;maa|VERB&gt; &lt;ne|DET&gt; &lt;kunu|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>31 &lt;Efei|ADV&gt; &lt;Ananse|PROPN&gt; &lt;see,|VERB&gt; &lt;“Eno,|NOUN&gt; &lt;fa|VERB&gt; &lt;aduane|NOUN&gt; &lt;si|VERB&gt; &lt;me|PRON&gt; &lt;so.”|ADV&gt;</t>
+  </si>
+  <si>
+    <t>32 &lt;Aso|PROPN&gt; &lt;de|VERB&gt; &lt;bi|DET&gt; &lt;sii|VERB&gt; &lt;so,|ADV&gt; &lt;na|CONJ&gt; &lt;Ananse|PROPN&gt; &lt;bisaa|VERB&gt; &lt;se,|SCONJ&gt; &lt;“Eno,|NOUN&gt; &lt;fufuo|NOUN&gt; &lt;na|CONJ&gt; &lt;wonoa|VERB&gt; &lt;anaa|CONJ&gt; &lt;eto?”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>34 &lt;Ananse|PROPN&gt; &lt;see,|VERB&gt; &lt;“Ene|ADV&gt; &lt;esua;|VERB&gt; &lt;k?fa|VERB&gt; &lt;kukuo|NOUN&gt; &lt;k?se.”|ADJ&gt;</t>
+  </si>
+  <si>
+    <t>35 &lt;Aso|PROPN&gt; &lt;k?faa|VERB&gt; &lt;k?se,|ADJ&gt; &lt;na|CONJ&gt; &lt;Ananse|PROPN&gt; &lt;ka|VERB&gt; &lt;se,|SCONJ&gt; &lt;“Bra|VERB&gt; &lt;begye|VERB&gt; &lt;nam.”|NOUN&gt; &lt;W?w?|VERB&gt; &lt;mmoa|NOUN&gt; &lt;ak?se|ADJ&gt; &lt;de?|PRON&gt; &lt;asere|VERB&gt; &lt;aduanan|NUM&gt;</t>
+  </si>
+  <si>
+    <t>36 &lt;?see,|VERB&gt; &lt;“Fa|VERB&gt; &lt;eyi|DET&gt; &lt;nko|ADV&gt; &lt;to|VERB&gt; &lt;mu,|PRON&gt; &lt;na|CONJ&gt; &lt;s?|SCONJ&gt; &lt;wow?|VERB&gt; &lt;kukuo|NOUN&gt; &lt;k?se|ADJ&gt; &lt;a,|SCONJ&gt; &lt;anka|ADV&gt; &lt;mede|VERB&gt; &lt;nam|NOUN&gt; &lt;bebubu|VERB&gt; &lt;w’aso.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>37 &lt;Aso|PROPN&gt; &lt;wiee|VERB&gt; &lt;aduane|NOUN&gt; &lt;no,|PRON&gt; &lt;guu|VERB&gt; &lt;so,|ADV&gt; &lt;de|VERB&gt; &lt;sii|VERB&gt; &lt;pon|NOUN&gt; &lt;so,|ADV&gt; &lt;hui|VERB&gt; &lt;nsuo,|NOUN&gt; &lt;na|CONJ&gt; &lt;?de|VERB&gt; &lt;sii|VERB&gt; &lt;h?|ADV&gt;</t>
+  </si>
+  <si>
+    <t>38 &lt;Na|CONJ&gt; &lt;Aso|PROPN&gt; &lt;faa|VERB&gt; &lt;ne|DET&gt; &lt;dea|NOUN&gt; &lt;k?t??|VERB&gt; &lt;ogya|NOUN&gt; &lt;ho,|ADV&gt; &lt;na|CONJ&gt; &lt;mmarima|NOUN&gt; &lt;no|DET&gt; &lt;k?tenaa|VERB&gt; &lt;pon|NOUN&gt; &lt;no|PRON&gt; &lt;ho|ADV&gt;</t>
+  </si>
+  <si>
+    <t>39 &lt;Na|CONJ&gt; &lt;y?kaa|VERB&gt; &lt;y?n|PRON&gt; &lt;nsa|NOUN&gt; &lt;akyi|ADV&gt;</t>
+  </si>
+  <si>
+    <t>40 &lt;Y?redi,|VERB&gt; &lt;y?redi,|VERB&gt; &lt;Kwaku|PROPN&gt; &lt;Ananse|PROPN&gt; &lt;kae|VERB&gt; &lt;se,|SCONJ&gt; &lt;“Fufuo|NOUN&gt; &lt;yi,|PRON&gt; &lt;nkyene|NOUN&gt; &lt;nni|VERB&gt; &lt;mu.”|ADP&gt;</t>
+  </si>
+  <si>
+    <t>41 &lt;Akwasi|PROPN&gt; &lt;ka|VERB&gt; &lt;kyer??|VERB&gt; &lt;Aso|PROPN&gt; &lt;se,|SCONJ&gt; &lt;“Fa|VERB&gt; &lt;bi|DET&gt; &lt;bra.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>42 &lt;Nanso|CONJ&gt; &lt;Ananse|PROPN&gt; &lt;see,|VERB&gt; &lt;“Dabi,|INTJ&gt; &lt;?baa|NOUN&gt; &lt;no|PRON&gt; &lt;redidi|VERB&gt; &lt;a,|SCONJ&gt; &lt;wo|PRON&gt; &lt;ka|VERB&gt; &lt;se|SCONJ&gt; &lt;?nsore|VERB&gt; &lt;nk?fa|VERB&gt; &lt;nkyene,|NOUN&gt; &lt;na|CONJ&gt; &lt;wo|PRON&gt; &lt;ara|ADV&gt; &lt;k?fa|VERB&gt; &lt;bra.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>43 &lt;Akwasi|PROPN&gt; &lt;s?ree,|VERB&gt; &lt;na|CONJ&gt; &lt;Ananse|PROPN&gt; &lt;hwehw??|VERB&gt; &lt;ne|DET&gt; &lt;to|NOUN&gt; &lt;mu,|PRON&gt; &lt;na|CONJ&gt; &lt;?faa|VERB&gt; &lt;aduro|NOUN&gt; &lt;guu|VERB&gt; &lt;fufuo|NOUN&gt; &lt;no|PRON&gt; &lt;mu|ADV&gt;</t>
+  </si>
+  <si>
+    <t>44 &lt;Efei|ADV&gt; &lt;?fr??|VERB&gt; &lt;Akwasi|PROPN&gt; &lt;se,|SCONJ&gt; &lt;“Bra|VERB&gt; &lt;na|CONJ&gt; &lt;nkyene|NOUN&gt; &lt;a|PART&gt; &lt;mede|VERB&gt; &lt;bae.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>45 &lt;Akwasi|PROPN&gt; &lt;bae,|VERB&gt; &lt;Ananse|PROPN&gt; &lt;see,|VERB&gt; &lt;“O,|INTJ&gt; &lt;meredi|VERB&gt; &lt;bio|ADV&gt; &lt;daabi,|INTJ&gt; &lt;mame.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>46 &lt;Akwasi|PROPN&gt; &lt;a|PART&gt; &lt;wannim|VERB&gt; &lt;hwee|PRON&gt; &lt;no|PRON&gt; &lt;toaa|VERB&gt; &lt;didi|NOUN&gt; &lt;no|PRON&gt; &lt;so,|ADV&gt; &lt;?dii|VERB&gt; &lt;na|CONJ&gt; &lt;?dii|VERB&gt;</t>
+  </si>
+  <si>
+    <t>47 &lt;Y?wiee|VERB&gt; &lt;didi|NOUN&gt; &lt;no,|PRON&gt; &lt;Akwasi|PROPN&gt; &lt;kae|VERB&gt; &lt;se,|SCONJ&gt; &lt;“Damfo,|NOUN&gt; &lt;y?ne|PRON&gt; &lt;wo|PRON&gt; &lt;te|VERB&gt; &lt;ha|ADV&gt; &lt;nanso|CONJ&gt; &lt;y?nnim|VERB&gt; &lt;wo|DET&gt; &lt;din.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>48 &lt;Ananse|PROPN&gt; &lt;see,|VERB&gt; &lt;“Me|PRON&gt; &lt;din|NOUN&gt; &lt;de|VERB&gt; &lt;‘Sore-ko-di-Aso.’”|PROPN&gt;</t>
+  </si>
+  <si>
+    <t>49 &lt;Akwasi|PROPN&gt; &lt;see,|VERB&gt; &lt;“Mate,|VERB&gt; &lt;Aso,|PROPN&gt; &lt;wote|VERB&gt; &lt;saa|ADV&gt; &lt;barima|NOUN&gt; &lt;yi|PRON&gt; &lt;din?”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>50 &lt;Aso|PROPN&gt; &lt;see,|VERB&gt; &lt;“Ei,|INTJ&gt; &lt;matie.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>51 &lt;Akwasi|PROPN&gt; &lt;s?ree|VERB&gt; &lt;k?|VERB&gt; &lt;siesiee|VERB&gt; &lt;adamp?n|NOUN&gt; &lt;baako|DET&gt; &lt;kama|ADV&gt;</t>
+  </si>
+  <si>
+    <t>52 &lt;?see,|VERB&gt; &lt;“Sore-ko-di-Aso,|PROPN&gt; &lt;wo|PRON&gt; &lt;dampon|NOUN&gt; &lt;ni,|PRON&gt; &lt;k?|VERB&gt; &lt;da|VERB&gt; &lt;ho.”|ADV&gt;</t>
+  </si>
+  <si>
+    <t>53 &lt;Ananse|PROPN&gt; &lt;see,|VERB&gt; &lt;“Mey?|VERB&gt; &lt;Nyankop?n|PROPN&gt; &lt;kra|NOUN&gt; &lt;dwara,|NOUN&gt; &lt;me|PRON&gt; &lt;da|VERB&gt; &lt;patom’.|NOUN&gt; &lt;Efi|ADV&gt; &lt;s?|SCONJ&gt; &lt;me|PRON&gt; &lt;maame|NOUN&gt; &lt;ne|CONJ&gt; &lt;me|PRON&gt; &lt;papa|NOUN&gt; &lt;woo|VERB&gt; &lt;me,|PRON&gt; &lt;meny?|VERB&gt; &lt;da|NOUN&gt; &lt;dampon|NOUN&gt; &lt;mu.”|ADV&gt;</t>
+  </si>
+  <si>
+    <t>54 &lt;Akwasi|PROPN&gt; &lt;see,|VERB&gt; &lt;“Na|CONJ&gt; &lt;?he|ADV&gt; &lt;na|CONJ&gt; &lt;w’ada?”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>55 &lt;?see,|VERB&gt; &lt;“S?|SCONJ&gt; &lt;mede|VERB&gt; &lt;meho|PRON&gt; &lt;b?da|VERB&gt; &lt;patom’|NOUN&gt; &lt;yi|PRON&gt; &lt;mu|ADV&gt; &lt;a,|SCONJ&gt; &lt;anka|ADV&gt; &lt;?kyer?|VERB&gt; &lt;se|SCONJ&gt; &lt;wo|PRON&gt; &lt;ne|DET&gt; &lt;Nyankop?n|PROPN&gt; &lt;bo|NOUN&gt; &lt;din.|VERB&gt; &lt;Meyere|VERB&gt; &lt;da|NOUN&gt; &lt;Nyankop?n|PROPN&gt; &lt;patom’|NOUN&gt; &lt;nka|VERB&gt; &lt;obiara|PRON&gt; &lt;de?.|PART&gt; &lt;Na|CONJ&gt; &lt;enti|ADV&gt; &lt;dampon|NOUN&gt; &lt;a|PART&gt; &lt;woda|VERB&gt; &lt;no|PRON&gt; &lt;anim|NOUN&gt; &lt;na|CONJ&gt; &lt;mede|VERB&gt; &lt;m’adan.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>56 &lt;?barima|NOUN&gt; &lt;no|PRON&gt; &lt;yii|VERB&gt; &lt;mpa|NOUN&gt; &lt;bi|DET&gt; &lt;too|VERB&gt; &lt;h?.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>57 &lt;Akwasi|PROPN&gt; &lt;ne|DET&gt; &lt;ne|PRON&gt; &lt;yere|NOUN&gt; &lt;k?daa,|VERB&gt; &lt;na|CONJ&gt; &lt;Ananse|PROPN&gt; &lt;nso|ADV&gt; &lt;daa|VERB&gt; &lt;h?.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>58 &lt;Ananse|PROPN&gt; &lt;daa|VERB&gt; &lt;h?,|ADV&gt; &lt;na|CONJ&gt; &lt;?kyea|VERB&gt; &lt;anomaa.|NOUN&gt; &lt;Ananse|PROPN&gt; &lt;daa|VERB&gt; &lt;h?|ADV&gt; &lt;na|CONJ&gt; &lt;?faa|VERB&gt; &lt;ne|DET&gt; &lt;sepirewa|NOUN&gt; &lt;kae:|VERB&gt;</t>
+  </si>
+  <si>
+    <t>59 &lt;“Akuamoa|PROPN&gt; &lt;Ananse,|PROPN&gt; &lt;?nn?|ADV&gt; &lt;yeb?y?|VERB&gt; &lt;biribi|NOUN&gt; &lt;?nn?.|ADV&gt; &lt;Nyame|PROPN&gt; &lt;de,|VERB&gt; &lt;Nsia|PROPN&gt; &lt;ba|NOUN&gt; &lt;Ananse,|PROPN&gt; &lt;?nn?|ADV&gt; &lt;yeb?y?|VERB&gt; &lt;biribi|NOUN&gt; &lt;?nn?.|ADV&gt; &lt;Nyame|PROPN&gt; &lt;kradwarefo|NOUN&gt; &lt;Ananse,|PROPN&gt; &lt;?nn?|ADV&gt; &lt;mehunu|VERB&gt; &lt;biribi.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>60 &lt;Efei|ADV&gt; &lt;ogyaee|VERB&gt; &lt;sepirewa|NOUN&gt; &lt;no,|PRON&gt; &lt;na|CONJ&gt; &lt;?de|VERB&gt; &lt;too|VERB&gt; &lt;h?,|ADV&gt; &lt;na|CONJ&gt; &lt;?daaa.|VERB&gt;</t>
+  </si>
+  <si>
+    <t>61 &lt;?da|VERB&gt; &lt;kakra,|ADV&gt; &lt;?tee|VERB&gt; &lt;Akwasi|PROPN&gt; &lt;Ninkunfuo|PROPN&gt; &lt;refr?|VERB&gt; &lt;no,|PRON&gt; &lt;“Agya|NOUN&gt; &lt;Barima.”|NOUN&gt; &lt;Dinn!|INTJ&gt;</t>
+  </si>
+  <si>
+    <t>62 &lt;“Agya|NOUN&gt; &lt;Barima.”|NOUN&gt; &lt;Dinn!|INTJ&gt;</t>
+  </si>
+  <si>
+    <t>63 &lt;Akwasi|PROPN&gt; &lt;Ninkunfuo|PROPN&gt; &lt;res?e;|VERB&gt; &lt;aduro|NOUN&gt; &lt;no|PRON&gt; &lt;akyekyere|VERB&gt; &lt;no,|PRON&gt; &lt;nanso|CONJ&gt; &lt;?fr?|VERB&gt; &lt;“Agya|NOUN&gt; &lt;Barima.”|NOUN&gt; &lt;Dinn!|INTJ&gt;</t>
+  </si>
+  <si>
+    <t>64 &lt;Afei|ADV&gt; &lt;?kae|VERB&gt; &lt;se,|SCONJ&gt; &lt;“Sore-ko-di-Aso.”|PROPN&gt;</t>
+  </si>
+  <si>
+    <t>65 &lt;?see,|VERB&gt; &lt;“M!|INTJ&gt; &lt;M!|INTJ&gt; &lt;M!”|INTJ&gt;</t>
+  </si>
+  <si>
+    <t>66 &lt;?see,|VERB&gt; &lt;“Bue|VERB&gt; &lt;me.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>67 &lt;Ananse|PROPN&gt; &lt;buee|VERB&gt; &lt;no,|PRON&gt; &lt;na|CONJ&gt; &lt;Akwasi|PROPN&gt; &lt;k??|VERB&gt; &lt;baabi.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>68 &lt;Afei|ADV&gt; &lt;Ananse|PROPN&gt; &lt;s?ree|VERB&gt; &lt;k??|VERB&gt; &lt;adan|NOUN&gt; &lt;no|PRON&gt; &lt;ho.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>69 &lt;?see,|VERB&gt; &lt;“Aso,|PROPN&gt; &lt;w’ate|VERB&gt; &lt;nea|PRON&gt; &lt;wo|DET&gt; &lt;kunu|NOUN&gt; &lt;aka?”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>70 &lt;?kae|VERB&gt; &lt;se,|SCONJ&gt; &lt;“Osee|VERB&gt; &lt;d?n?”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>71 &lt;?see,|VERB&gt; &lt;“Osee|VERB&gt; &lt;mennsore|VERB&gt; &lt;mmedi|VERB&gt; &lt;wo.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>73 &lt;Na|CONJ&gt; &lt;?y?|VERB&gt; &lt;maa|VERB&gt; &lt;no,|PRON&gt; &lt;na|CONJ&gt; &lt;?san|VERB&gt; &lt;k?daa.|VERB&gt;</t>
+  </si>
+  <si>
+    <t>74 &lt;Anadwo|NOUN&gt; &lt;no,|PRON&gt; &lt;Akwasi|PROPN&gt; &lt;soree|VERB&gt; &lt;mp?n|NUM&gt; &lt;nkr?n;|NUM&gt; &lt;Ananse|PROPN&gt; &lt;nso|ADV&gt; &lt;k??|VERB&gt; &lt;Aso|PROPN&gt; &lt;nky?n|NOUN&gt; &lt;mp?n|NUM&gt; &lt;nkr?n.|NUM&gt;</t>
+  </si>
+  <si>
+    <t>75 &lt;Ade|NOUN&gt; &lt;kyee|VERB&gt; &lt;an?pa,|ADV&gt; &lt;Ananse|PROPN&gt; &lt;s?ree|VERB&gt; &lt;k?e.|VERB&gt;</t>
+  </si>
+  <si>
+    <t>76 &lt;Nna|ADV&gt; &lt;ebia|ADV&gt; &lt;asram|NUM&gt; &lt;mmienu,|NUM&gt; &lt;na|CONJ&gt; &lt;Aso|PROPN&gt; &lt;yafunu|NOUN&gt; &lt;ab?.|VERB&gt;</t>
+  </si>
+  <si>
+    <t>77 &lt;Akwasi|PROPN&gt; &lt;bisaa|VERB&gt; &lt;no|PRON&gt; &lt;se,|SCONJ&gt; &lt;“Ad?n|PRON&gt; &lt;na|CONJ&gt; &lt;wo|PRON&gt; &lt;yafunu|NOUN&gt; &lt;ab?|VERB&gt; &lt;saa,|ADV&gt; &lt;ebia|ADV&gt; &lt;woyare,|VERB&gt; &lt;na|CONJ&gt; &lt;me|PRON&gt; &lt;a|PART&gt; &lt;mete|VERB&gt; &lt;wo|PRON&gt; &lt;ho|ADV&gt; &lt;no,|PRON&gt; &lt;mennyin|VERB&gt; &lt;ba.”|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>78 &lt;Aso|PROPN&gt; &lt;see,|VERB&gt; &lt;“Wo|PRON&gt; &lt;wer?|VERB&gt; &lt;afi|VERB&gt; &lt;onipa|NOUN&gt; &lt;no|PRON&gt; &lt;a|PART&gt; &lt;?baa|VERB&gt; &lt;ha|ADV&gt; &lt;no|PRON&gt; &lt;a|PART&gt; &lt;wokae|VERB&gt; &lt;se,|SCONJ&gt; &lt;‘Sore-ko-di-Aso’?|PROPN&gt; &lt;?no|PRON&gt; &lt;na|CONJ&gt; &lt;ofaa|VERB&gt; &lt;me|PRON&gt; &lt;na|CONJ&gt; &lt;?ne|PRON&gt; &lt;me|PRON&gt; &lt;nyem.”|VERB&gt;</t>
+  </si>
+  <si>
+    <t>79 &lt;Akwasi|PROPN&gt; &lt;Ninkunfuo|PROPN&gt; &lt;see,|VERB&gt; &lt;“Sore|VERB&gt; &lt;ma|VERB&gt; &lt;menfa|VERB&gt; &lt;wo|PRON&gt; &lt;nk?|VERB&gt; &lt;ne|DET&gt; &lt;nky?n.”|ADV&gt;</t>
+  </si>
+  <si>
+    <t>80 &lt;Y?k??|VERB&gt; &lt;Nyankop?n|PROPN&gt; &lt;kurom’.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>81 &lt;W?|VERB&gt; &lt;kwan|NOUN&gt; &lt;so|ADV&gt; &lt;Aso|PROPN&gt; &lt;woo|VERB&gt; &lt;babi.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>82 &lt;Y?duruu|VERB&gt; &lt;Nyame|PROPN&gt; &lt;kurom’|NOUN&gt; &lt;kaa|VERB&gt; &lt;amanne|NOUN&gt; &lt;se,|SCONJ&gt; &lt;“Wo|PRON&gt; &lt;akoa|NOUN&gt; &lt;bi|DET&gt; &lt;a|PART&gt; &lt;wasoma|VERB&gt; &lt;no|PRON&gt; &lt;a|PART&gt; &lt;?daa|VERB&gt; &lt;me|PRON&gt; &lt;fie,|NOUN&gt; &lt;ofaa|VERB&gt; &lt;Aso|PROPN&gt; &lt;na|CONJ&gt; &lt;?ny??|VERB&gt; &lt;no.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>83 &lt;Nyankop?n|PROPN&gt; &lt;see,|VERB&gt; &lt;“Me|PRON&gt; &lt;nkoa|NOUN&gt; &lt;nyinaa|PRON&gt; &lt;reb?|VERB&gt; &lt;dan|NOUN&gt; &lt;atifi,|ADV&gt; &lt;k?kyer?|VERB&gt; &lt;onipa|NOUN&gt; &lt;koro|ADJ&gt; &lt;no.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>84 &lt;Y?k?e,|VERB&gt; &lt;na|CONJ&gt; &lt;Ananse|PROPN&gt; &lt;te|VERB&gt; &lt;etire|NOUN&gt; &lt;so.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>86 &lt;Na|CONJ&gt; &lt;Ananse|PROPN&gt; &lt;de|VERB&gt; &lt;gyae|VERB&gt; &lt;k?tenaa|VERB&gt; &lt;mfinmfini.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>87 &lt;Na|CONJ&gt; &lt;Aso|PROPN&gt; &lt;san|VERB&gt; &lt;kae|VERB&gt; &lt;se,|SCONJ&gt; &lt;“O’nie.”|INTJ&gt;</t>
+  </si>
+  <si>
+    <t>88 &lt;Afei|ADV&gt; &lt;Ananse|PROPN&gt; &lt;firi|VERB&gt; &lt;soro|NOUN&gt; &lt;h?|ADV&gt; &lt;b??|VERB&gt; &lt;fam.|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>89 &lt;Da|NOUN&gt; &lt;no|DET&gt; &lt;so,|ADV&gt; &lt;eye|VERB&gt; &lt;Fiada.|PROPN&gt;</t>
+  </si>
+  <si>
+    <t>90 &lt;Ananse|PROPN&gt; &lt;see,|VERB&gt; &lt;“Me|PRON&gt; &lt;dware|VERB&gt; &lt;kra|NOUN&gt; &lt;na|CONJ&gt; &lt;wo|PRON&gt; &lt;de|VERB&gt; &lt;wo|DET&gt; &lt;nsa|NOUN&gt; &lt;kyer??|VERB&gt; &lt;me|PRON&gt; &lt;so,|ADV&gt; &lt;maa|VERB&gt; &lt;meb??|VERB&gt; &lt;fam|NOUN&gt; &lt;hunu.”|ADV&gt;</t>
+  </si>
+  <si>
+    <t>91 &lt;Seesei|ADV&gt; &lt;na|CONJ&gt; &lt;nhenkwa|NOUN&gt; &lt;hy??|VERB&gt; &lt;Akwasi|PROPN&gt; &lt;Ninkunfuo|PROPN&gt; &lt;mu,|PRON&gt; &lt;na|CONJ&gt; &lt;?twaa|VERB&gt; &lt;odwan|NOUN&gt;</t>
+  </si>
+  <si>
+    <t>92 &lt;Akwasi|PROPN&gt; &lt;Ninkunfuo|PROPN&gt; &lt;twaa|VERB&gt; &lt;odwan|NOUN&gt; &lt;no|PRON&gt; &lt;wiee,|ADV&gt; &lt;?ka|VERB&gt; &lt;kyer??|VERB&gt; &lt;Nyame|PROPN&gt; &lt;se,|SCONJ&gt; &lt;“Obaa|NOUN&gt; &lt;yi|PRON&gt; &lt;ni,|INTJ&gt; &lt;ma|VERB&gt; &lt;Ananse|PROPN&gt; &lt;nfa|VERB&gt; &lt;no.”|PRON&gt;</t>
+  </si>
+  <si>
+    <t>93 &lt;Ananse|PROPN&gt; &lt;faa|VERB&gt; &lt;Aso,|PROPN&gt; &lt;na|CONJ&gt; &lt;abofra|NOUN&gt; &lt;no|PRON&gt; &lt;de?|PRON&gt; &lt;wokum|VERB&gt; &lt;no|PRON&gt; &lt;twiwtaa|VERB&gt; &lt;n’nam|NOUN&gt; &lt;gyaa|VERB&gt; &lt;h?.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>94 &lt;?no|PRON&gt; &lt;ne|VERB&gt; &lt;?b?y?|VERB&gt; &lt;a|PART&gt; &lt;animguase|NOUN&gt; &lt;b?ba|VERB&gt; &lt;man|NOUN&gt; &lt;no|PRON&gt; &lt;mu.|ADV&gt;</t>
+  </si>
+  <si>
+    <t>95 &lt;Me|PRON&gt; &lt;ananses?m|NOUN&gt; &lt;a|PART&gt; &lt;metoo|VERB&gt; &lt;yi,|PRON&gt; &lt;s?|SCONJ&gt; &lt;eye|VERB&gt; &lt;de|VERB&gt; &lt;a,|SCONJ&gt; &lt;s?|SCONJ&gt; &lt;ennye|VERB&gt; &lt;de|VERB&gt; &lt;a,|SCONJ&gt; &lt;momfa|VERB&gt; &lt;bi|DET&gt; &lt;nko,|ADV&gt; &lt;na|CONJ&gt; &lt;momfa|VERB&gt; &lt;bi|DET&gt; &lt;mmera.|VERB&gt;</t>
   </si>
 </sst>
 </file>
@@ -1897,22 +2752,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F81895BA-2848-455B-905A-C745B19A29EF}">
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H97" sqref="H97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="56.7265625" customWidth="1"/>
-    <col min="2" max="2" width="62.90625" customWidth="1"/>
-    <col min="3" max="3" width="55.26953125" customWidth="1"/>
-    <col min="4" max="4" width="46.81640625" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" customWidth="1"/>
+    <col min="4" max="4" width="39.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" customWidth="1"/>
+    <col min="6" max="6" width="18.08984375" customWidth="1"/>
+    <col min="7" max="7" width="21.1796875" customWidth="1"/>
+    <col min="8" max="8" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1928,8 +2786,17 @@
       <c r="E1" s="1" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
@@ -1945,8 +2812,17 @@
       <c r="E2" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>475</v>
+      </c>
+      <c r="G2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H2" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1962,8 +2838,17 @@
       <c r="E3" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>476</v>
+      </c>
+      <c r="G3" t="s">
+        <v>572</v>
+      </c>
+      <c r="H3" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>45</v>
       </c>
@@ -1979,8 +2864,17 @@
       <c r="E4" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>477</v>
+      </c>
+      <c r="G4" t="s">
+        <v>573</v>
+      </c>
+      <c r="H4" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1996,8 +2890,17 @@
       <c r="E5" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>478</v>
+      </c>
+      <c r="G5" t="s">
+        <v>574</v>
+      </c>
+      <c r="H5" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -2013,8 +2916,17 @@
       <c r="E6" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>479</v>
+      </c>
+      <c r="G6" t="s">
+        <v>575</v>
+      </c>
+      <c r="H6" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -2030,8 +2942,17 @@
       <c r="E7" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>480</v>
+      </c>
+      <c r="G7" t="s">
+        <v>576</v>
+      </c>
+      <c r="H7" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>47</v>
       </c>
@@ -2047,8 +2968,17 @@
       <c r="E8" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>481</v>
+      </c>
+      <c r="G8" t="s">
+        <v>577</v>
+      </c>
+      <c r="H8" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>49</v>
       </c>
@@ -2064,8 +2994,17 @@
       <c r="E9" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>482</v>
+      </c>
+      <c r="G9" t="s">
+        <v>578</v>
+      </c>
+      <c r="H9" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
@@ -2081,8 +3020,17 @@
       <c r="E10" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>483</v>
+      </c>
+      <c r="G10" t="s">
+        <v>579</v>
+      </c>
+      <c r="H10" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>53</v>
       </c>
@@ -2098,8 +3046,17 @@
       <c r="E11" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>484</v>
+      </c>
+      <c r="G11" t="s">
+        <v>580</v>
+      </c>
+      <c r="H11" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>55</v>
       </c>
@@ -2115,8 +3072,17 @@
       <c r="E12" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>485</v>
+      </c>
+      <c r="G12" t="s">
+        <v>581</v>
+      </c>
+      <c r="H12" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -2132,8 +3098,17 @@
       <c r="E13" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>486</v>
+      </c>
+      <c r="G13" t="s">
+        <v>582</v>
+      </c>
+      <c r="H13" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>56</v>
       </c>
@@ -2149,8 +3124,17 @@
       <c r="E14" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>487</v>
+      </c>
+      <c r="G14" t="s">
+        <v>583</v>
+      </c>
+      <c r="H14" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -2166,8 +3150,17 @@
       <c r="E15" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>488</v>
+      </c>
+      <c r="G15" t="s">
+        <v>584</v>
+      </c>
+      <c r="H15" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>58</v>
       </c>
@@ -2183,8 +3176,17 @@
       <c r="E16" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>489</v>
+      </c>
+      <c r="G16" t="s">
+        <v>585</v>
+      </c>
+      <c r="H16" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>59</v>
       </c>
@@ -2200,8 +3202,17 @@
       <c r="E17" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>490</v>
+      </c>
+      <c r="G17" t="s">
+        <v>586</v>
+      </c>
+      <c r="H17" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>61</v>
       </c>
@@ -2217,8 +3228,17 @@
       <c r="E18" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>491</v>
+      </c>
+      <c r="G18" t="s">
+        <v>587</v>
+      </c>
+      <c r="H18" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
@@ -2234,8 +3254,17 @@
       <c r="E19" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F19" t="s">
+        <v>492</v>
+      </c>
+      <c r="G19" t="s">
+        <v>588</v>
+      </c>
+      <c r="H19" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>65</v>
       </c>
@@ -2251,8 +3280,17 @@
       <c r="E20" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F20" t="s">
+        <v>493</v>
+      </c>
+      <c r="G20" t="s">
+        <v>589</v>
+      </c>
+      <c r="H20" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>67</v>
       </c>
@@ -2268,8 +3306,17 @@
       <c r="E21" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F21" t="s">
+        <v>494</v>
+      </c>
+      <c r="G21" t="s">
+        <v>590</v>
+      </c>
+      <c r="H21" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
@@ -2285,8 +3332,17 @@
       <c r="E22" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>496</v>
+      </c>
+      <c r="G22" t="s">
+        <v>592</v>
+      </c>
+      <c r="H22" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>70</v>
       </c>
@@ -2302,8 +3358,17 @@
       <c r="E23" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F23" t="s">
+        <v>497</v>
+      </c>
+      <c r="G23" t="s">
+        <v>593</v>
+      </c>
+      <c r="H23" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>72</v>
       </c>
@@ -2319,8 +3384,17 @@
       <c r="E24" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>498</v>
+      </c>
+      <c r="G24" t="s">
+        <v>594</v>
+      </c>
+      <c r="H24" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>74</v>
       </c>
@@ -2336,8 +3410,17 @@
       <c r="E25" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F25" t="s">
+        <v>499</v>
+      </c>
+      <c r="G25" t="s">
+        <v>595</v>
+      </c>
+      <c r="H25" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>75</v>
       </c>
@@ -2353,8 +3436,17 @@
       <c r="E26" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F26" t="s">
+        <v>500</v>
+      </c>
+      <c r="G26" t="s">
+        <v>596</v>
+      </c>
+      <c r="H26" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>77</v>
       </c>
@@ -2370,8 +3462,17 @@
       <c r="E27" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" t="s">
+        <v>501</v>
+      </c>
+      <c r="G27" t="s">
+        <v>597</v>
+      </c>
+      <c r="H27" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>79</v>
       </c>
@@ -2387,8 +3488,17 @@
       <c r="E28" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F28" t="s">
+        <v>502</v>
+      </c>
+      <c r="G28" t="s">
+        <v>598</v>
+      </c>
+      <c r="H28" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>81</v>
       </c>
@@ -2404,8 +3514,17 @@
       <c r="E29" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F29" t="s">
+        <v>503</v>
+      </c>
+      <c r="G29" t="s">
+        <v>599</v>
+      </c>
+      <c r="H29" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>17</v>
       </c>
@@ -2421,8 +3540,17 @@
       <c r="E30" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30" t="s">
+        <v>504</v>
+      </c>
+      <c r="G30" t="s">
+        <v>600</v>
+      </c>
+      <c r="H30" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>84</v>
       </c>
@@ -2438,8 +3566,17 @@
       <c r="E31" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31" t="s">
+        <v>505</v>
+      </c>
+      <c r="G31" t="s">
+        <v>601</v>
+      </c>
+      <c r="H31" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>86</v>
       </c>
@@ -2455,8 +3592,17 @@
       <c r="E32" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F32" t="s">
+        <v>506</v>
+      </c>
+      <c r="G32" t="s">
+        <v>602</v>
+      </c>
+      <c r="H32" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>88</v>
       </c>
@@ -2472,8 +3618,17 @@
       <c r="E33" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33" t="s">
+        <v>507</v>
+      </c>
+      <c r="G33" t="s">
+        <v>603</v>
+      </c>
+      <c r="H33" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>90</v>
       </c>
@@ -2489,8 +3644,17 @@
       <c r="E34" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34" t="s">
+        <v>508</v>
+      </c>
+      <c r="G34" t="s">
+        <v>604</v>
+      </c>
+      <c r="H34" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>92</v>
       </c>
@@ -2506,8 +3670,17 @@
       <c r="E35" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F35" t="s">
+        <v>509</v>
+      </c>
+      <c r="G35" t="s">
+        <v>605</v>
+      </c>
+      <c r="H35" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>94</v>
       </c>
@@ -2523,8 +3696,17 @@
       <c r="E36" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F36" t="s">
+        <v>510</v>
+      </c>
+      <c r="G36" t="s">
+        <v>606</v>
+      </c>
+      <c r="H36" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>96</v>
       </c>
@@ -2540,8 +3722,17 @@
       <c r="E37" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F37" t="s">
+        <v>511</v>
+      </c>
+      <c r="G37" t="s">
+        <v>607</v>
+      </c>
+      <c r="H37" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>98</v>
       </c>
@@ -2557,8 +3748,17 @@
       <c r="E38" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F38" t="s">
+        <v>512</v>
+      </c>
+      <c r="G38" t="s">
+        <v>608</v>
+      </c>
+      <c r="H38" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>100</v>
       </c>
@@ -2574,8 +3774,17 @@
       <c r="E39" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F39" t="s">
+        <v>513</v>
+      </c>
+      <c r="G39" t="s">
+        <v>609</v>
+      </c>
+      <c r="H39" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>102</v>
       </c>
@@ -2591,8 +3800,17 @@
       <c r="E40" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F40" t="s">
+        <v>514</v>
+      </c>
+      <c r="G40" t="s">
+        <v>610</v>
+      </c>
+      <c r="H40" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>104</v>
       </c>
@@ -2608,8 +3826,17 @@
       <c r="E41" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F41" t="s">
+        <v>515</v>
+      </c>
+      <c r="G41" t="s">
+        <v>611</v>
+      </c>
+      <c r="H41" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>106</v>
       </c>
@@ -2625,8 +3852,17 @@
       <c r="E42" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F42" t="s">
+        <v>516</v>
+      </c>
+      <c r="G42" t="s">
+        <v>612</v>
+      </c>
+      <c r="H42" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>108</v>
       </c>
@@ -2642,8 +3878,17 @@
       <c r="E43" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F43" t="s">
+        <v>517</v>
+      </c>
+      <c r="G43" t="s">
+        <v>624</v>
+      </c>
+      <c r="H43" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>110</v>
       </c>
@@ -2659,8 +3904,17 @@
       <c r="E44" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F44" t="s">
+        <v>518</v>
+      </c>
+      <c r="G44" t="s">
+        <v>613</v>
+      </c>
+      <c r="H44" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>112</v>
       </c>
@@ -2676,8 +3930,17 @@
       <c r="E45" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F45" t="s">
+        <v>519</v>
+      </c>
+      <c r="G45" t="s">
+        <v>614</v>
+      </c>
+      <c r="H45" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>114</v>
       </c>
@@ -2693,8 +3956,17 @@
       <c r="E46" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F46" t="s">
+        <v>520</v>
+      </c>
+      <c r="G46" t="s">
+        <v>615</v>
+      </c>
+      <c r="H46" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>116</v>
       </c>
@@ -2710,8 +3982,17 @@
       <c r="E47" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F47" t="s">
+        <v>521</v>
+      </c>
+      <c r="G47" t="s">
+        <v>616</v>
+      </c>
+      <c r="H47" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>118</v>
       </c>
@@ -2727,8 +4008,17 @@
       <c r="E48" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F48" t="s">
+        <v>522</v>
+      </c>
+      <c r="G48" t="s">
+        <v>617</v>
+      </c>
+      <c r="H48" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>120</v>
       </c>
@@ -2744,8 +4034,17 @@
       <c r="E49" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F49" t="s">
+        <v>523</v>
+      </c>
+      <c r="G49" t="s">
+        <v>625</v>
+      </c>
+      <c r="H49" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>122</v>
       </c>
@@ -2761,8 +4060,17 @@
       <c r="E50" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F50" t="s">
+        <v>524</v>
+      </c>
+      <c r="G50" t="s">
+        <v>626</v>
+      </c>
+      <c r="H50" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>124</v>
       </c>
@@ -2778,8 +4086,17 @@
       <c r="E51" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F51" t="s">
+        <v>525</v>
+      </c>
+      <c r="G51" t="s">
+        <v>627</v>
+      </c>
+      <c r="H51" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>126</v>
       </c>
@@ -2795,8 +4112,17 @@
       <c r="E52" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F52" t="s">
+        <v>526</v>
+      </c>
+      <c r="G52" t="s">
+        <v>618</v>
+      </c>
+      <c r="H52" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>128</v>
       </c>
@@ -2812,8 +4138,17 @@
       <c r="E53" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F53" t="s">
+        <v>527</v>
+      </c>
+      <c r="G53" t="s">
+        <v>628</v>
+      </c>
+      <c r="H53" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>130</v>
       </c>
@@ -2829,8 +4164,17 @@
       <c r="E54" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F54" t="s">
+        <v>528</v>
+      </c>
+      <c r="G54" t="s">
+        <v>629</v>
+      </c>
+      <c r="H54" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>132</v>
       </c>
@@ -2846,8 +4190,17 @@
       <c r="E55" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="F55" t="s">
+        <v>529</v>
+      </c>
+      <c r="G55" t="s">
+        <v>619</v>
+      </c>
+      <c r="H55" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>134</v>
       </c>
@@ -2863,8 +4216,17 @@
       <c r="E56" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F56" t="s">
+        <v>547</v>
+      </c>
+      <c r="G56" t="s">
+        <v>630</v>
+      </c>
+      <c r="H56" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>136</v>
       </c>
@@ -2880,8 +4242,17 @@
       <c r="E57" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F57" t="s">
+        <v>530</v>
+      </c>
+      <c r="G57" t="s">
+        <v>620</v>
+      </c>
+      <c r="H57" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>138</v>
       </c>
@@ -2897,8 +4268,17 @@
       <c r="E58" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F58" t="s">
+        <v>531</v>
+      </c>
+      <c r="G58" t="s">
+        <v>621</v>
+      </c>
+      <c r="H58" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>140</v>
       </c>
@@ -2914,8 +4294,17 @@
       <c r="E59" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F59" t="s">
+        <v>532</v>
+      </c>
+      <c r="G59" t="s">
+        <v>622</v>
+      </c>
+      <c r="H59" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>142</v>
       </c>
@@ -2931,8 +4320,17 @@
       <c r="E60" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F60" t="s">
+        <v>533</v>
+      </c>
+      <c r="G60" t="s">
+        <v>631</v>
+      </c>
+      <c r="H60" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>144</v>
       </c>
@@ -2948,8 +4346,17 @@
       <c r="E61" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F61" t="s">
+        <v>534</v>
+      </c>
+      <c r="G61" t="s">
+        <v>623</v>
+      </c>
+      <c r="H61" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>18</v>
       </c>
@@ -2965,8 +4372,17 @@
       <c r="E62" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F62" t="s">
+        <v>535</v>
+      </c>
+      <c r="G62" t="s">
+        <v>632</v>
+      </c>
+      <c r="H62" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>19</v>
       </c>
@@ -2982,8 +4398,17 @@
       <c r="E63" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F63" t="s">
+        <v>536</v>
+      </c>
+      <c r="G63" t="s">
+        <v>633</v>
+      </c>
+      <c r="H63" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>148</v>
       </c>
@@ -2999,8 +4424,17 @@
       <c r="E64" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F64" t="s">
+        <v>537</v>
+      </c>
+      <c r="G64" t="s">
+        <v>634</v>
+      </c>
+      <c r="H64" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>20</v>
       </c>
@@ -3016,8 +4450,17 @@
       <c r="E65" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F65" t="s">
+        <v>538</v>
+      </c>
+      <c r="G65" t="s">
+        <v>635</v>
+      </c>
+      <c r="H65" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>22</v>
       </c>
@@ -3033,8 +4476,17 @@
       <c r="E66" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F66" t="s">
+        <v>539</v>
+      </c>
+      <c r="G66" t="s">
+        <v>636</v>
+      </c>
+      <c r="H66" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>24</v>
       </c>
@@ -3050,8 +4502,17 @@
       <c r="E67" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F67" t="s">
+        <v>540</v>
+      </c>
+      <c r="G67" t="s">
+        <v>637</v>
+      </c>
+      <c r="H67" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>25</v>
       </c>
@@ -3067,8 +4528,17 @@
       <c r="E68" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F68" t="s">
+        <v>541</v>
+      </c>
+      <c r="G68" t="s">
+        <v>638</v>
+      </c>
+      <c r="H68" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>151</v>
       </c>
@@ -3084,8 +4554,17 @@
       <c r="E69" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F69" t="s">
+        <v>542</v>
+      </c>
+      <c r="G69" t="s">
+        <v>639</v>
+      </c>
+      <c r="H69" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>153</v>
       </c>
@@ -3101,8 +4580,17 @@
       <c r="E70" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F70" t="s">
+        <v>543</v>
+      </c>
+      <c r="G70" t="s">
+        <v>640</v>
+      </c>
+      <c r="H70" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>26</v>
       </c>
@@ -3118,8 +4606,17 @@
       <c r="E71" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F71" t="s">
+        <v>544</v>
+      </c>
+      <c r="G71" t="s">
+        <v>641</v>
+      </c>
+      <c r="H71" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>27</v>
       </c>
@@ -3135,8 +4632,17 @@
       <c r="E72" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F72" t="s">
+        <v>545</v>
+      </c>
+      <c r="G72" t="s">
+        <v>642</v>
+      </c>
+      <c r="H72" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>28</v>
       </c>
@@ -3152,8 +4658,17 @@
       <c r="E73" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F73" t="s">
+        <v>546</v>
+      </c>
+      <c r="G73" t="s">
+        <v>643</v>
+      </c>
+      <c r="H73" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>29</v>
       </c>
@@ -3169,8 +4684,17 @@
       <c r="E74" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F74" t="s">
+        <v>548</v>
+      </c>
+      <c r="G74" t="s">
+        <v>644</v>
+      </c>
+      <c r="H74" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>159</v>
       </c>
@@ -3186,8 +4710,17 @@
       <c r="E75" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F75" t="s">
+        <v>549</v>
+      </c>
+      <c r="G75" t="s">
+        <v>645</v>
+      </c>
+      <c r="H75" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>161</v>
       </c>
@@ -3203,8 +4736,17 @@
       <c r="E76" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F76" t="s">
+        <v>550</v>
+      </c>
+      <c r="G76" t="s">
+        <v>646</v>
+      </c>
+      <c r="H76" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>30</v>
       </c>
@@ -3220,8 +4762,17 @@
       <c r="E77" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F77" t="s">
+        <v>551</v>
+      </c>
+      <c r="G77" t="s">
+        <v>647</v>
+      </c>
+      <c r="H77" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>164</v>
       </c>
@@ -3237,8 +4788,17 @@
       <c r="E78" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F78" t="s">
+        <v>552</v>
+      </c>
+      <c r="G78" t="s">
+        <v>648</v>
+      </c>
+      <c r="H78" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>166</v>
       </c>
@@ -3254,8 +4814,17 @@
       <c r="E79" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F79" t="s">
+        <v>553</v>
+      </c>
+      <c r="G79" t="s">
+        <v>649</v>
+      </c>
+      <c r="H79" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>168</v>
       </c>
@@ -3271,8 +4840,17 @@
       <c r="E80" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F80" t="s">
+        <v>554</v>
+      </c>
+      <c r="G80" t="s">
+        <v>650</v>
+      </c>
+      <c r="H80" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>170</v>
       </c>
@@ -3288,8 +4866,17 @@
       <c r="E81" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F81" t="s">
+        <v>555</v>
+      </c>
+      <c r="G81" t="s">
+        <v>651</v>
+      </c>
+      <c r="H81" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>35</v>
       </c>
@@ -3305,8 +4892,17 @@
       <c r="E82" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F82" t="s">
+        <v>556</v>
+      </c>
+      <c r="G82" t="s">
+        <v>652</v>
+      </c>
+      <c r="H82" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>172</v>
       </c>
@@ -3322,8 +4918,17 @@
       <c r="E83" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F83" t="s">
+        <v>557</v>
+      </c>
+      <c r="G83" t="s">
+        <v>653</v>
+      </c>
+      <c r="H83" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>174</v>
       </c>
@@ -3339,8 +4944,17 @@
       <c r="E84" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F84" t="s">
+        <v>558</v>
+      </c>
+      <c r="G84" t="s">
+        <v>654</v>
+      </c>
+      <c r="H84" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>176</v>
       </c>
@@ -3356,8 +4970,17 @@
       <c r="E85" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F85" t="s">
+        <v>559</v>
+      </c>
+      <c r="G85" t="s">
+        <v>655</v>
+      </c>
+      <c r="H85" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
         <v>38</v>
       </c>
@@ -3373,8 +4996,17 @@
       <c r="E86" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F86" t="s">
+        <v>560</v>
+      </c>
+      <c r="G86" t="s">
+        <v>656</v>
+      </c>
+      <c r="H86" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>177</v>
       </c>
@@ -3390,8 +5022,17 @@
       <c r="E87" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F87" t="s">
+        <v>561</v>
+      </c>
+      <c r="G87" t="s">
+        <v>657</v>
+      </c>
+      <c r="H87" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
         <v>40</v>
       </c>
@@ -3407,8 +5048,17 @@
       <c r="E88" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F88" t="s">
+        <v>562</v>
+      </c>
+      <c r="G88" t="s">
+        <v>658</v>
+      </c>
+      <c r="H88" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>178</v>
       </c>
@@ -3424,8 +5074,17 @@
       <c r="E89" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F89" t="s">
+        <v>563</v>
+      </c>
+      <c r="G89" t="s">
+        <v>659</v>
+      </c>
+      <c r="H89" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>41</v>
       </c>
@@ -3441,8 +5100,17 @@
       <c r="E90" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F90" t="s">
+        <v>564</v>
+      </c>
+      <c r="G90" t="s">
+        <v>660</v>
+      </c>
+      <c r="H90" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>181</v>
       </c>
@@ -3458,8 +5126,17 @@
       <c r="E91" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F91" t="s">
+        <v>565</v>
+      </c>
+      <c r="G91" t="s">
+        <v>661</v>
+      </c>
+      <c r="H91" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
         <v>183</v>
       </c>
@@ -3475,8 +5152,17 @@
       <c r="E92" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F92" t="s">
+        <v>566</v>
+      </c>
+      <c r="G92" t="s">
+        <v>662</v>
+      </c>
+      <c r="H92" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
         <v>185</v>
       </c>
@@ -3492,8 +5178,17 @@
       <c r="E93" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F93" t="s">
+        <v>567</v>
+      </c>
+      <c r="G93" t="s">
+        <v>663</v>
+      </c>
+      <c r="H93" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>187</v>
       </c>
@@ -3509,8 +5204,17 @@
       <c r="E94" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F94" t="s">
+        <v>568</v>
+      </c>
+      <c r="G94" t="s">
+        <v>664</v>
+      </c>
+      <c r="H94" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>189</v>
       </c>
@@ -3526,8 +5230,17 @@
       <c r="E95" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F95" t="s">
+        <v>569</v>
+      </c>
+      <c r="G95" t="s">
+        <v>665</v>
+      </c>
+      <c r="H95" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
         <v>190</v>
       </c>
@@ -3542,6 +5255,15 @@
       </c>
       <c r="E96" t="s">
         <v>474</v>
+      </c>
+      <c r="F96" t="s">
+        <v>570</v>
+      </c>
+      <c r="G96" t="s">
+        <v>666</v>
+      </c>
+      <c r="H96" t="s">
+        <v>759</v>
       </c>
     </row>
   </sheetData>

</xml_diff>